<commit_message>
Updated spreadsheets to finmath-lib 4.0.6.
</commit_message>
<xml_diff>
--- a/spreadsheets/Caplets/Caplets.xlsx
+++ b/spreadsheets/Caplets/Caplets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Dokumente\Development\finmath spreadsheets\spreadsheets\Caplets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\finmath-spreadsheets\spreadsheets\Caplets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Load Libs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <calcPr calcId="152511" iterate="1" iterateCount="2" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -36,12 +36,22 @@
   <si>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Note:</t>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">This sheet requires Obba 4.0.14 or better ( </t>
     </r>
     <r>
       <rPr>
@@ -49,15 +59,6 @@
         <u/>
         <sz val="8"/>
         <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>This sheet requires Obba 4.0.14 or better (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -70,7 +71,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>)</t>
+      <t xml:space="preserve"> )</t>
     </r>
   </si>
   <si>
@@ -152,7 +153,7 @@
     <t>We then define a model containing all discount cuves and forward curves.</t>
   </si>
   <si>
-    <t/>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Curve Properties and Past Fixings</t>
@@ -269,7 +270,7 @@
     <t>end</t>
   </si>
   <si>
-    <t>quoting convention:</t>
+    <t xml:space="preserve">quoting convention: </t>
   </si>
   <si>
     <t>frequency</t>
@@ -351,15 +352,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-407];[Red]\-#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="165" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -489,9 +506,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -499,31 +524,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -550,10 +575,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -571,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -586,15 +611,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Erklärender Text" xfId="1" builtinId="53" customBuiltin="1"/>
+  <cellStyles count="6">
+    <cellStyle name="Excel Built-in Title" xfId="5"/>
+    <cellStyle name="Heading" xfId="3"/>
+    <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Result" xfId="1"/>
+    <cellStyle name="Result2" xfId="2"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -687,9 +716,9 @@
     <definedNames>
       <definedName name="OBADDALLJARS"/>
       <definedName name="OBADDCLASSES"/>
-      <definedName name="OBCALL"/>
-      <definedName name="OBCONTROLPANELSETVISIBLE"/>
-      <definedName name="OBGET"/>
+      <definedName name="obCall"/>
+      <definedName name="obControlPanelSetVisible"/>
+      <definedName name="obGet"/>
       <definedName name="OBGETPROPERTY"/>
       <definedName name="obMake"/>
     </definedNames>
@@ -969,16 +998,16 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.08984375" style="1"/>
-    <col min="4" max="7" width="10.7265625" style="1"/>
-    <col min="8" max="8" width="18.7265625" style="1"/>
-    <col min="9" max="10" width="10.7265625" style="1"/>
-    <col min="11" max="11" width="11.7265625" style="1"/>
-    <col min="12" max="12" width="10.7265625" style="2"/>
-    <col min="13" max="256" width="10.7265625" style="1"/>
-    <col min="257" max="1025" width="11.54296875"/>
+    <col min="1" max="3" width="9.109375" style="1" customWidth="1"/>
+    <col min="4" max="7" width="10.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="2" customWidth="1"/>
+    <col min="13" max="256" width="10.6640625" style="1" customWidth="1"/>
+    <col min="257" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1041,7 +1070,7 @@
     </row>
     <row r="11" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="b">
-        <f>[1]!OBCONTROLPANELSETVISIBLE(C8)</f>
+        <f>[1]!obControlPanelSetVisible(C8)</f>
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -1055,7 +1084,7 @@
       </c>
       <c r="F12" s="1" t="str">
         <f>[1]!OBADDALLJARS(F8,F9)</f>
-        <v>Z:\Dokumente\Development\finmath spreadsheets\spreadsheets\Caplets\lib</v>
+        <v>\\vmware-host\Shared Folders\finmath-spreadsheets\spreadsheets\Caplets\lib</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1084,7 +1113,7 @@
       </c>
       <c r="C17" s="1" t="str">
         <f>[1]!OBGETPROPERTY("version")</f>
-        <v>4.2.2</v>
+        <v>6.1.0</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>6</v>
@@ -1097,7 +1126,7 @@
       </c>
       <c r="C18" s="1" t="str">
         <f>[1]!OBGETPROPERTY("build")</f>
-        <v>40201</v>
+        <v>60100</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>8</v>
@@ -1123,7 +1152,7 @@
       </c>
       <c r="F21" s="1" t="str">
         <f>[1]!OBADDCLASSES(F17,F18)</f>
-        <v>Z:\Dokumente\Development\finmath spreadsheets\spreadsheets\Caplets\</v>
+        <v>\\vmware-host\Shared Folders\finmath-spreadsheets\spreadsheets\Caplets\</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1137,8 +1166,8 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="str">
-        <f>[1]!OBGET([1]!OBCALL("",obLibs&amp;"net.finmath.information.Library","getVersionString"))</f>
-        <v>2.0.0</v>
+        <f>[1]!obGet([1]!obCall("",obLibs&amp;"net.finmath.information.Library","getVersionString"))</f>
+        <v>4.0.6-SNAPSHOT</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1155,7 +1184,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1167,18 +1196,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" style="12"/>
-    <col min="2" max="230" width="14.26953125" style="12"/>
-    <col min="231" max="1025" width="14.26953125"/>
+    <col min="1" max="1" width="5.109375" style="12" customWidth="1"/>
+    <col min="2" max="230" width="14.33203125" style="12" customWidth="1"/>
+    <col min="231" max="1025" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:1024" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:1024" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="HW1" s="12"/>
       <c r="HX1" s="12"/>
     </row>
@@ -1199,9 +1226,9 @@
     </row>
     <row r="3" spans="2:1024" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="16" t="str">
-        <f>[1]!obMake("referenceDate "&amp;COLUMN(),obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",G3))</f>
+        <f>[1]!obMake("referenceDate "&amp;COLUMN(),"LocalDate",G3)</f>
         <v>referenceDate 6 
-[12967]</v>
+[6074]</v>
       </c>
       <c r="G3" s="17">
         <v>40918</v>
@@ -1243,14 +1270,14 @@
     </row>
     <row r="8" spans="2:1024" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="str">
-        <f>[1]!obMake("modelWithDiscountingCurve",obLibs&amp;"net.finmath.marketdata.model.AnalyticModel",[1]!obMake("",obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterface[]",B28))</f>
+        <f>[1]!obMake("modelWithDiscountingCurve",obLibs&amp;"net.finmath.marketdata.model.AnalyticModelFromCurvesAndVols",[1]!obMake("",obLibs&amp;"net.finmath.marketdata.model.curves.Curve[]",B28))</f>
         <v>modelWithDiscountingCurve 
-[13077]</v>
+[6252]</v>
       </c>
       <c r="F8" s="16" t="str">
-        <f>[1]!obMake("modelWithForwardAndDiscountingCurves",obLibs&amp;"net.finmath.marketdata.model.AnalyticModel",[1]!obMake("",obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterface[]",B28,F28,J28))</f>
+        <f>[1]!obMake("modelWithForwardAndDiscountingCurves",obLibs&amp;"net.finmath.marketdata.model.AnalyticModelFromCurvesAndVols",[1]!obMake("",obLibs&amp;"net.finmath.marketdata.model.curves.Curve[]",B28,F28,J28))</f>
         <v>modelWithForwardAndDiscountingCurves 
-[13240]</v>
+[6435]</v>
       </c>
       <c r="I8" s="15"/>
     </row>
@@ -1267,10 +1294,10 @@
       <c r="I10" s="15" t="str">
         <f>"To use these curves as reference the cell containing the modell name "&amp;F8</f>
         <v>To use these curves as reference the cell containing the modell name modelWithForwardAndDiscountingCurves 
-[13240]</v>
-      </c>
-    </row>
-    <row r="12" spans="2:1024" s="20" customFormat="1" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+[6435]</v>
+      </c>
+    </row>
+    <row r="12" spans="2:1024" s="20" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
         <v>28</v>
       </c>
@@ -1303,7 +1330,7 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="14" spans="2:1024" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:1024" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
         <v>29</v>
       </c>
@@ -1320,8 +1347,8 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="2:1024" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:1024" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:1024" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:1024" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>30</v>
       </c>
@@ -1338,7 +1365,7 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>31</v>
       </c>
@@ -1358,11 +1385,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="str">
-        <f>[1]!OBCALL("interpolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$InterpolationMethod","valueOf",[1]!obMake("","String",C18))</f>
+    <row r="18" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="str">
+        <f>[1]!obCall("interpolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$InterpolationMethod","valueOf",[1]!obMake("","String",C18))</f>
         <v>interpolationMethod 2 
-[13031]</v>
+[6144]</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>35</v>
@@ -1370,7 +1397,7 @@
       <c r="F18" s="16" t="str">
         <f>[1]!obMake("indexMaturity "&amp;COLUMN(),"String",G18)</f>
         <v>indexMaturity 6 
-[12953]</v>
+[6073]</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>36</v>
@@ -1378,17 +1405,17 @@
       <c r="J18" s="16" t="str">
         <f>[1]!obMake("indexMaturity "&amp;COLUMN(),"String",K18)</f>
         <v>indexMaturity 10 
-[12914]</v>
+[6085]</v>
       </c>
       <c r="K18" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="str">
-        <f>[1]!OBCALL("extrapolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$ExtrapolationMethod","valueOf",[1]!obMake("","String",C19))</f>
+    <row r="19" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="str">
+        <f>[1]!obCall("extrapolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$ExtrapolationMethod","valueOf",[1]!obMake("","String",C19))</f>
         <v>extrapolationMethod 2 
-[13007]</v>
+[6112]</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>38</v>
@@ -1396,7 +1423,7 @@
       <c r="F19" s="16" t="str">
         <f>[1]!obMake("businessDayCal "&amp;COLUMN(),obLibs&amp;"net.finmath.time.businessdaycalendar."&amp;G19)</f>
         <v>businessDayCal 6 
-[13026]</v>
+[6118]</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>39</v>
@@ -1404,120 +1431,120 @@
       <c r="J19" s="16" t="str">
         <f>[1]!obMake("businessDayCal "&amp;COLUMN(),obLibs&amp;"net.finmath.time.businessdaycalendar."&amp;K19)</f>
         <v>businessDayCal 10 
-[13027]</v>
+[6150]</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="str">
-        <f>[1]!OBCALL("interpolationEntity "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$InterpolationEntity","valueOf",[1]!obMake("","String",C20))</f>
+    <row r="20" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="str">
+        <f>[1]!obCall("interpolationEntity "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$InterpolationEntity","valueOf",[1]!obMake("","String",C20))</f>
         <v>interpolationEntity 2 
-[13055]</v>
+[6185]</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="16" t="str">
-        <f>[1]!OBCALL("dayCountConvention"&amp;COLUMN(),obLibs&amp;"net.finmath.time.businessdaycalendar.BusinessdayCalendarInterface$DateRollConvention","valueOf",[1]!obMake("","String",G20))</f>
+        <f>[1]!obCall("dayCountConvention"&amp;COLUMN(),obLibs&amp;"net.finmath.time.businessdaycalendar.BusinessdayCalendar$DateRollConvention","valueOf",[1]!obMake("","String",G20))</f>
         <v>dayCountConvention6 
-[12971]</v>
+[6181]</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>41</v>
       </c>
       <c r="J20" s="16" t="str">
-        <f>[1]!OBCALL("dayCountConvention"&amp;COLUMN(),obLibs&amp;"net.finmath.time.businessdaycalendar.BusinessdayCalendarInterface$DateRollConvention","valueOf",[1]!obMake("","String",K20))</f>
+        <f>[1]!obCall("dayCountConvention"&amp;COLUMN(),obLibs&amp;"net.finmath.time.businessdaycalendar.BusinessdayCalendar$DateRollConvention","valueOf",[1]!obMake("","String",K20))</f>
         <v>dayCountConvention10 
-[12991]</v>
+[6091]</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="16"/>
-      <c r="F21" s="16" t="str">
-        <f>[1]!OBCALL("interpolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$InterpolationMethod","valueOf",[1]!obMake("","String",G21))</f>
+      <c r="F21" s="19" t="str">
+        <f>[1]!obCall("interpolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$InterpolationMethod","valueOf",[1]!obMake("","String",G21))</f>
         <v>interpolationMethod 6 
-[13033]</v>
+[6140]</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="J21" s="16" t="str">
-        <f>[1]!OBCALL("interpolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$InterpolationMethod","valueOf",[1]!obMake("","String",K21))</f>
+      <c r="J21" s="19" t="str">
+        <f>[1]!obCall("interpolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$InterpolationMethod","valueOf",[1]!obMake("","String",K21))</f>
         <v>interpolationMethod 10 
-[13061]</v>
+[6127]</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="16"/>
-      <c r="F22" s="16" t="str">
-        <f>[1]!OBCALL("extrapolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$ExtrapolationMethod","valueOf",[1]!obMake("","String",G22))</f>
+      <c r="F22" s="19" t="str">
+        <f>[1]!obCall("extrapolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$ExtrapolationMethod","valueOf",[1]!obMake("","String",G22))</f>
         <v>extrapolationMethod 6 
-[13044]</v>
+[6196]</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="J22" s="16" t="str">
-        <f>[1]!OBCALL("extrapolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$ExtrapolationMethod","valueOf",[1]!obMake("","String",K22))</f>
+      <c r="J22" s="19" t="str">
+        <f>[1]!obCall("extrapolationMethod "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$ExtrapolationMethod","valueOf",[1]!obMake("","String",K22))</f>
         <v>extrapolationMethod 10 
-[12964]</v>
+[6087]</v>
       </c>
       <c r="K22" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="16"/>
-      <c r="F23" s="16" t="str">
-        <f>[1]!OBCALL("interpolationEntity "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$InterpolationEntity","valueOf",[1]!obMake("","String",G23))</f>
+      <c r="F23" s="19" t="str">
+        <f>[1]!obCall("interpolationEntity "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$InterpolationEntity","valueOf",[1]!obMake("","String",G23))</f>
         <v>interpolationEntity 6 
-[13011]</v>
+[6110]</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="16" t="str">
-        <f>[1]!OBCALL("interpolationEntity "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.Curve$InterpolationEntity","valueOf",[1]!obMake("","String",K23))</f>
+      <c r="J23" s="19" t="str">
+        <f>[1]!obCall("interpolationEntity "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.CurveInterpolation$InterpolationEntity","valueOf",[1]!obMake("","String",K23))</f>
         <v>interpolationEntity 10 
-[12987]</v>
+[6148]</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="16"/>
       <c r="F24" s="16" t="str">
-        <f>[1]!OBCALL("forwardInterpolationEntity"&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurve$InterpolationEntityForward","valueOf",[1]!obMake("","String",G24))</f>
+        <f>[1]!obCall("forwardInterpolationEntity"&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurveInterpolation$InterpolationEntityForward","valueOf",[1]!obMake("","String",G24))</f>
         <v>forwardInterpolationEntity6 
-[13068]</v>
+[6146]</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="16" t="str">
-        <f>[1]!OBCALL("forwardInterpolationEntity"&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurve$InterpolationEntityForward","valueOf",[1]!obMake("","String",K24))</f>
+        <f>[1]!obCall("forwardInterpolationEntity"&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurveInterpolation$InterpolationEntityForward","valueOf",[1]!obMake("","String",K24))</f>
         <v>forwardInterpolationEntity10 
-[13029]</v>
+[6142]</v>
       </c>
       <c r="K24" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="16"/>
       <c r="F25" s="16" t="str">
         <f>[1]!obMake("discountCurve"&amp;COLUMN(),"String",G25)</f>
         <v>discountCurve6 
-[12920]</v>
+[6072]</v>
       </c>
       <c r="G25" s="21" t="str">
         <f>C17</f>
@@ -1526,21 +1553,21 @@
       <c r="J25" s="16" t="str">
         <f>[1]!obMake("discountCurve"&amp;COLUMN(),"String",K25)</f>
         <v>discountCurve10 
-[12887]</v>
+[6084]</v>
       </c>
       <c r="K25" s="21" t="str">
         <f>G17</f>
         <v>forward-EUR-3M</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
     </row>
-    <row r="27" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>45</v>
       </c>
@@ -1557,26 +1584,26 @@
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
     </row>
-    <row r="28" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="str">
-        <f>[1]!OBCALL("curveObject-"&amp;C17&amp;"-curveDef",obLibs&amp;"net.finmath.marketdata.model.curves.DiscountCurve","createDiscountCurveFromZeroRates",[1]!obMake("","String",C17),F3,[1]!obMake("","double[]",C31:C351),[1]!obMake("","double[]",D31:D351),B18:B20)</f>
+        <f>[1]!obCall("curveObject-"&amp;C17&amp;"-curveDef",obLibs&amp;"net.finmath.marketdata.model.curves.DiscountCurveInterpolation","createDiscountCurveFromZeroRates",[1]!obMake("","String",C17),F3,[1]!obMake("","double[]",C31:C351),[1]!obMake("","double[]",D31:D351),B18:B20)</f>
         <v>curveObject-discount-EUR-OIS-curveDef 
-[13059]</v>
+[6189]</v>
       </c>
       <c r="C28" s="22"/>
       <c r="F28" s="16" t="str">
-        <f>[1]!OBCALL(G17,obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurve","createForwardCurveFromForwards",[1]!obMake("","String",G17),$F$3,[1]!obMake("","String",G18),F19:F24,[1]!obMake("","String",F25),B8,[1]!obMake("","double[]",G31:G351),[1]!obMake("","double[]",H31:H351))</f>
+        <f>[1]!obCall(G17,obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurveInterpolation","createForwardCurveFromForwards",[1]!obMake("","String",G17),$F$3,[1]!obMake("","String",G18),F19:F24,[1]!obMake("","String",F25),B8,[1]!obMake("","double[]",G31:G351),[1]!obMake("","double[]",H31:H351))</f>
         <v>forward-EUR-3M 
-[13179]</v>
+[6321]</v>
       </c>
       <c r="J28" s="16" t="str">
-        <f>[1]!OBCALL(K17,obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurve","createForwardCurveFromForwards",[1]!obMake("","String",K17),$F$3,[1]!obMake("","String",K18),J19:J24,[1]!obMake("","String",J25),B8,[1]!obMake("","double[]",K31:K351),[1]!obMake("","double[]",L31:L351))</f>
+        <f>[1]!obCall(K17,obLibs&amp;"net.finmath.marketdata.model.curves.ForwardCurveInterpolation","createForwardCurveFromForwards",[1]!obMake("","String",K17),$F$3,[1]!obMake("","String",K18),J19:J24,[1]!obMake("","String",J25),B8,[1]!obMake("","double[]",K31:K351),[1]!obMake("","double[]",L31:L351))</f>
         <v>forward-EUR-6M 
-[13173]</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+[6315]</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
         <v>47</v>
       </c>
@@ -1605,7 +1632,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24">
         <v>40917</v>
       </c>
@@ -1634,7 +1661,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="24">
         <v>40916</v>
       </c>
@@ -1663,7 +1690,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="24">
         <v>40915</v>
       </c>
@@ -1692,7 +1719,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="24">
         <v>40914</v>
       </c>
@@ -1750,7 +1777,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="24">
         <v>40912</v>
       </c>
@@ -1779,7 +1806,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="24">
         <v>40911</v>
       </c>
@@ -1808,7 +1835,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="24">
         <v>40910</v>
       </c>
@@ -1837,7 +1864,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="24">
         <v>40909</v>
       </c>
@@ -1866,7 +1893,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="24">
         <v>40908</v>
       </c>
@@ -1895,7 +1922,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="24">
         <v>40907</v>
       </c>
@@ -1924,7 +1951,7 @@
         <v>6.0870280686755596E-3</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="24">
         <v>40906</v>
       </c>
@@ -1953,7 +1980,7 @@
         <v>6.1323577793989002E-3</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="24">
         <v>40905</v>
       </c>
@@ -1982,7 +2009,7 @@
         <v>6.1817468672019597E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="24">
         <v>40904</v>
       </c>
@@ -2011,7 +2038,7 @@
         <v>6.2311359550050096E-3</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="24">
         <v>40903</v>
       </c>
@@ -2040,7 +2067,7 @@
         <v>6.2805250428080604E-3</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="24">
         <v>40902</v>
       </c>
@@ -2069,7 +2096,7 @@
         <v>6.3299141306111103E-3</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="24">
         <v>40901</v>
       </c>
@@ -2098,7 +2125,7 @@
         <v>6.3793032184141603E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="24">
         <v>40900</v>
       </c>
@@ -2127,7 +2154,7 @@
         <v>6.4286923062172102E-3</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="24">
         <v>40899</v>
       </c>
@@ -2156,7 +2183,7 @@
         <v>6.4780813940202601E-3</v>
       </c>
     </row>
-    <row r="50" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="24">
         <v>40898</v>
       </c>
@@ -2185,7 +2212,7 @@
         <v>6.52747048182331E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="24">
         <v>40897</v>
       </c>
@@ -2214,7 +2241,7 @@
         <v>6.57685956962636E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="24">
         <v>40896</v>
       </c>
@@ -2243,7 +2270,7 @@
         <v>6.6262486574294099E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="24">
         <v>40895</v>
       </c>
@@ -2272,7 +2299,7 @@
         <v>6.6756377452324702E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="24">
         <v>40894</v>
       </c>
@@ -2301,7 +2328,7 @@
         <v>6.7250268330355202E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="24">
         <v>40893</v>
       </c>
@@ -2330,7 +2357,7 @@
         <v>6.7744159208385701E-3</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="24">
         <v>40892</v>
       </c>
@@ -2359,7 +2386,7 @@
         <v>6.82380500864162E-3</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="24">
         <v>40891</v>
       </c>
@@ -2388,7 +2415,7 @@
         <v>6.87319409644467E-3</v>
       </c>
     </row>
-    <row r="58" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="24">
         <v>40890</v>
       </c>
@@ -2417,7 +2444,7 @@
         <v>6.9225831842477199E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="24">
         <v>40889</v>
       </c>
@@ -2446,7 +2473,7 @@
         <v>6.9719722720507698E-3</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="24">
         <v>40888</v>
       </c>
@@ -2475,7 +2502,7 @@
         <v>7.0213613598538198E-3</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="24">
         <v>40887</v>
       </c>
@@ -2504,7 +2531,7 @@
         <v>7.0707504476568697E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="24">
         <v>40886</v>
       </c>
@@ -2533,7 +2560,7 @@
         <v>7.1781024427321899E-3</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="24">
         <v>40885</v>
       </c>
@@ -2562,7 +2589,7 @@
         <v>7.29064514592144E-3</v>
       </c>
     </row>
-    <row r="64" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="24">
         <v>40884</v>
       </c>
@@ -2591,7 +2618,7 @@
         <v>7.4031878491106901E-3</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="24">
         <v>40883</v>
       </c>
@@ -2620,7 +2647,7 @@
         <v>7.5157305522999401E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="24">
         <v>40882</v>
       </c>
@@ -2649,7 +2676,7 @@
         <v>7.6282732554891902E-3</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="24">
         <v>40881</v>
       </c>
@@ -2678,7 +2705,7 @@
         <v>7.7408159586784498E-3</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="24">
         <v>40880</v>
       </c>
@@ -2707,7 +2734,7 @@
         <v>7.8533586618677008E-3</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="24">
         <v>40879</v>
       </c>
@@ -2736,7 +2763,7 @@
         <v>7.9659013650569491E-3</v>
       </c>
     </row>
-    <row r="70" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="24">
         <v>40878</v>
       </c>
@@ -2765,7 +2792,7 @@
         <v>8.0784440682461992E-3</v>
       </c>
     </row>
-    <row r="71" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="24">
         <v>40877</v>
       </c>
@@ -2794,7 +2821,7 @@
         <v>8.1909867714354493E-3</v>
       </c>
     </row>
-    <row r="72" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="24">
         <v>40876</v>
       </c>
@@ -2823,7 +2850,7 @@
         <v>8.3035294746246994E-3</v>
       </c>
     </row>
-    <row r="73" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="24">
         <v>40875</v>
       </c>
@@ -2852,7 +2879,7 @@
         <v>8.4160721778139495E-3</v>
       </c>
     </row>
-    <row r="74" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="24">
         <v>40874</v>
       </c>
@@ -2881,7 +2908,7 @@
         <v>8.5286148810031995E-3</v>
       </c>
     </row>
-    <row r="75" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="24">
         <v>40873</v>
       </c>
@@ -2910,7 +2937,7 @@
         <v>8.6411575841924496E-3</v>
       </c>
     </row>
-    <row r="76" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="24">
         <v>40872</v>
       </c>
@@ -2939,7 +2966,7 @@
         <v>8.7537002873816997E-3</v>
       </c>
     </row>
-    <row r="77" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="24">
         <v>40871</v>
       </c>
@@ -2968,7 +2995,7 @@
         <v>8.8662429905709602E-3</v>
       </c>
     </row>
-    <row r="78" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="24">
         <v>40870</v>
       </c>
@@ -2997,7 +3024,7 @@
         <v>8.9787856937602103E-3</v>
       </c>
     </row>
-    <row r="79" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="24">
         <v>40869</v>
       </c>
@@ -3026,7 +3053,7 @@
         <v>9.0913283969494604E-3</v>
       </c>
     </row>
-    <row r="80" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="24">
         <v>40868</v>
       </c>
@@ -3055,7 +3082,7 @@
         <v>9.2038711001387104E-3</v>
       </c>
     </row>
-    <row r="81" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="24">
         <v>40867</v>
       </c>
@@ -3084,7 +3111,7 @@
         <v>9.3164138033279605E-3</v>
       </c>
     </row>
-    <row r="82" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="24">
         <v>40866</v>
       </c>
@@ -3113,7 +3140,7 @@
         <v>9.5127035850662706E-3</v>
       </c>
     </row>
-    <row r="83" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="24">
         <v>40865</v>
       </c>
@@ -3142,7 +3169,7 @@
         <v>9.72886555493486E-3</v>
       </c>
     </row>
-    <row r="84" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="24">
         <v>40864</v>
       </c>
@@ -3171,7 +3198,7 @@
         <v>9.9450275248034493E-3</v>
       </c>
     </row>
-    <row r="85" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="24">
         <v>40863</v>
       </c>
@@ -3200,7 +3227,7 @@
         <v>1.0161189494672001E-2</v>
       </c>
     </row>
-    <row r="86" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="24">
         <v>40862</v>
       </c>
@@ -3229,7 +3256,7 @@
         <v>1.03773514645406E-2</v>
       </c>
     </row>
-    <row r="87" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="24">
         <v>40861</v>
       </c>
@@ -3258,7 +3285,7 @@
         <v>1.05935134344092E-2</v>
       </c>
     </row>
-    <row r="88" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="24">
         <v>40860</v>
       </c>
@@ -3287,7 +3314,7 @@
         <v>1.08096754042778E-2</v>
       </c>
     </row>
-    <row r="89" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="24">
         <v>40859</v>
       </c>
@@ -3316,7 +3343,7 @@
         <v>1.10258373741464E-2</v>
       </c>
     </row>
-    <row r="90" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="24">
         <v>40858</v>
       </c>
@@ -3345,7 +3372,7 @@
         <v>1.1241999344015E-2</v>
       </c>
     </row>
-    <row r="91" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="24">
         <v>40857</v>
       </c>
@@ -3374,7 +3401,7 @@
         <v>1.1458161313883599E-2</v>
       </c>
     </row>
-    <row r="92" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="24">
         <v>40856</v>
       </c>
@@ -3403,7 +3430,7 @@
         <v>1.1674323283752199E-2</v>
       </c>
     </row>
-    <row r="93" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="24">
         <v>40855</v>
       </c>
@@ -3432,7 +3459,7 @@
         <v>1.1890485253620801E-2</v>
       </c>
     </row>
-    <row r="94" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="24">
         <v>40854</v>
       </c>
@@ -3461,7 +3488,7 @@
         <v>1.21066472234894E-2</v>
       </c>
     </row>
-    <row r="95" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="24">
         <v>40853</v>
       </c>
@@ -3490,7 +3517,7 @@
         <v>1.2322809193358E-2</v>
       </c>
     </row>
-    <row r="96" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="24">
         <v>40852</v>
       </c>
@@ -3519,7 +3546,7 @@
         <v>1.25389711632266E-2</v>
       </c>
     </row>
-    <row r="97" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="24">
         <v>40851</v>
       </c>
@@ -3548,7 +3575,7 @@
         <v>1.2755133133095099E-2</v>
       </c>
     </row>
-    <row r="98" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="24">
         <v>40850</v>
       </c>
@@ -3577,7 +3604,7 @@
         <v>1.2971295102963701E-2</v>
       </c>
     </row>
-    <row r="99" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="24">
         <v>40849</v>
       </c>
@@ -3606,7 +3633,7 @@
         <v>1.3187457072832301E-2</v>
       </c>
     </row>
-    <row r="100" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="24">
         <v>40848</v>
       </c>
@@ -3635,7 +3662,7 @@
         <v>1.34036190427009E-2</v>
       </c>
     </row>
-    <row r="101" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="24">
         <v>40847</v>
       </c>
@@ -3664,7 +3691,7 @@
         <v>1.36197810125695E-2</v>
       </c>
     </row>
-    <row r="102" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="24">
         <v>40846</v>
       </c>
@@ -3693,7 +3720,7 @@
         <v>1.3803956051706701E-2</v>
       </c>
     </row>
-    <row r="103" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="24">
         <v>40845</v>
       </c>
@@ -3722,7 +3749,7 @@
         <v>1.39830538002516E-2</v>
       </c>
     </row>
-    <row r="104" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="24">
         <v>40844</v>
       </c>
@@ -3751,7 +3778,7 @@
         <v>1.4162151548796501E-2</v>
       </c>
     </row>
-    <row r="105" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="24">
         <v>40843</v>
       </c>
@@ -3780,7 +3807,7 @@
         <v>1.43412492973414E-2</v>
       </c>
     </row>
-    <row r="106" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="24">
         <v>40842</v>
       </c>
@@ -3809,7 +3836,7 @@
         <v>1.4520347045886201E-2</v>
       </c>
     </row>
-    <row r="107" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="24">
         <v>40841</v>
       </c>
@@ -3838,7 +3865,7 @@
         <v>1.46994447944311E-2</v>
       </c>
     </row>
-    <row r="108" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="24">
         <v>40840</v>
       </c>
@@ -3867,7 +3894,7 @@
         <v>1.4878542542976001E-2</v>
       </c>
     </row>
-    <row r="109" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="24">
         <v>40839</v>
       </c>
@@ -3896,7 +3923,7 @@
         <v>1.50576402915209E-2</v>
       </c>
     </row>
-    <row r="110" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="24">
         <v>40838</v>
       </c>
@@ -3925,7 +3952,7 @@
         <v>1.5236738040065799E-2</v>
       </c>
     </row>
-    <row r="111" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="24">
         <v>40837</v>
       </c>
@@ -3954,7 +3981,7 @@
         <v>1.54158357886107E-2</v>
       </c>
     </row>
-    <row r="112" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="24">
         <v>40836</v>
       </c>
@@ -3983,7 +4010,7 @@
         <v>1.5594933537155501E-2</v>
       </c>
     </row>
-    <row r="113" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="24">
         <v>40835</v>
       </c>
@@ -4012,7 +4039,7 @@
         <v>1.5774031285700402E-2</v>
       </c>
     </row>
-    <row r="114" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="24">
         <v>40834</v>
       </c>
@@ -4041,7 +4068,7 @@
         <v>1.5953129034245301E-2</v>
       </c>
     </row>
-    <row r="115" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="24">
         <v>40833</v>
       </c>
@@ -4070,7 +4097,7 @@
         <v>1.61322267827902E-2</v>
       </c>
     </row>
-    <row r="116" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="24">
         <v>40832</v>
       </c>
@@ -4099,7 +4126,7 @@
         <v>1.6311324531335099E-2</v>
       </c>
     </row>
-    <row r="117" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="24">
         <v>40831</v>
       </c>
@@ -4128,7 +4155,7 @@
         <v>1.6490422279879999E-2</v>
       </c>
     </row>
-    <row r="118" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="24">
         <v>40830</v>
       </c>
@@ -4157,7 +4184,7 @@
         <v>1.6669520028424901E-2</v>
       </c>
     </row>
-    <row r="119" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="24">
         <v>40829</v>
       </c>
@@ -4186,7 +4213,7 @@
         <v>1.68486177769697E-2</v>
       </c>
     </row>
-    <row r="120" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="24">
         <v>40828</v>
       </c>
@@ -4215,7 +4242,7 @@
         <v>1.7027715525514599E-2</v>
       </c>
     </row>
-    <row r="121" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="24">
         <v>40827</v>
       </c>
@@ -4244,7 +4271,7 @@
         <v>1.7206813274059499E-2</v>
       </c>
     </row>
-    <row r="122" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="24">
         <v>40826</v>
       </c>
@@ -4273,7 +4300,7 @@
         <v>1.7428754340267999E-2</v>
       </c>
     </row>
-    <row r="123" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="24">
         <v>40825</v>
       </c>
@@ -4302,7 +4329,7 @@
         <v>1.7657495933089701E-2</v>
       </c>
     </row>
-    <row r="124" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="24">
         <v>40824</v>
       </c>
@@ -4331,7 +4358,7 @@
         <v>1.7886237525911401E-2</v>
       </c>
     </row>
-    <row r="125" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="24">
         <v>40823</v>
       </c>
@@ -4360,7 +4387,7 @@
         <v>1.81149791187331E-2</v>
       </c>
     </row>
-    <row r="126" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="24">
         <v>40822</v>
       </c>
@@ -4389,7 +4416,7 @@
         <v>1.8343720711554799E-2</v>
       </c>
     </row>
-    <row r="127" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="24">
         <v>40821</v>
       </c>
@@ -4418,7 +4445,7 @@
         <v>1.8572462304376602E-2</v>
       </c>
     </row>
-    <row r="128" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="24">
         <v>40820</v>
       </c>
@@ -4447,7 +4474,7 @@
         <v>1.8801203897198301E-2</v>
       </c>
     </row>
-    <row r="129" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="24">
         <v>40819</v>
       </c>
@@ -4476,7 +4503,7 @@
         <v>1.902994549002E-2</v>
       </c>
     </row>
-    <row r="130" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="24">
         <v>40818</v>
       </c>
@@ -4505,7 +4532,7 @@
         <v>1.9258687082841699E-2</v>
       </c>
     </row>
-    <row r="131" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="24">
         <v>40817</v>
       </c>
@@ -4534,7 +4561,7 @@
         <v>1.9487428675663401E-2</v>
       </c>
     </row>
-    <row r="132" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="24">
         <v>40816</v>
       </c>
@@ -4563,7 +4590,7 @@
         <v>1.9716170268485201E-2</v>
       </c>
     </row>
-    <row r="133" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="24">
         <v>40815</v>
       </c>
@@ -4592,7 +4619,7 @@
         <v>1.99449118613069E-2</v>
       </c>
     </row>
-    <row r="134" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="24">
         <v>40814</v>
       </c>
@@ -4621,7 +4648,7 @@
         <v>2.0173653454128599E-2</v>
       </c>
     </row>
-    <row r="135" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="24">
         <v>40813</v>
       </c>
@@ -4650,7 +4677,7 @@
         <v>2.0402395046950302E-2</v>
       </c>
     </row>
-    <row r="136" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="24">
         <v>40812</v>
       </c>
@@ -4679,7 +4706,7 @@
         <v>2.0631136639772001E-2</v>
       </c>
     </row>
-    <row r="137" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="24">
         <v>40811</v>
       </c>
@@ -4708,7 +4735,7 @@
         <v>2.08598782325937E-2</v>
       </c>
     </row>
-    <row r="138" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="24">
         <v>40810</v>
       </c>
@@ -4737,7 +4764,7 @@
         <v>2.1088619825415499E-2</v>
       </c>
     </row>
-    <row r="139" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="24">
         <v>40809</v>
       </c>
@@ -4766,7 +4793,7 @@
         <v>2.1317361418237198E-2</v>
       </c>
     </row>
-    <row r="140" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="24">
         <v>40808</v>
       </c>
@@ -4795,7 +4822,7 @@
         <v>2.1546103011058901E-2</v>
       </c>
     </row>
-    <row r="141" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="24">
         <v>40807</v>
       </c>
@@ -4824,7 +4851,7 @@
         <v>2.17748446038806E-2</v>
       </c>
     </row>
-    <row r="142" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="24">
         <v>40806</v>
       </c>
@@ -4853,7 +4880,7 @@
         <v>2.1884836244998301E-2</v>
       </c>
     </row>
-    <row r="143" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="24">
         <v>40805</v>
       </c>
@@ -4882,7 +4909,7 @@
         <v>2.1975978687432899E-2</v>
       </c>
     </row>
-    <row r="144" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="24">
         <v>40804</v>
       </c>
@@ -4911,7 +4938,7 @@
         <v>2.20671211298674E-2</v>
       </c>
     </row>
-    <row r="145" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="24">
         <v>40803</v>
       </c>
@@ -4940,7 +4967,7 @@
         <v>2.2158263572301901E-2</v>
       </c>
     </row>
-    <row r="146" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="24">
         <v>40802</v>
       </c>
@@ -4969,7 +4996,7 @@
         <v>2.2249406014736399E-2</v>
       </c>
     </row>
-    <row r="147" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="24">
         <v>40801</v>
       </c>
@@ -4998,7 +5025,7 @@
         <v>2.2340548457171001E-2</v>
       </c>
     </row>
-    <row r="148" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="24">
         <v>40800</v>
       </c>
@@ -5027,7 +5054,7 @@
         <v>2.2431690899605498E-2</v>
       </c>
     </row>
-    <row r="149" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="24">
         <v>40799</v>
       </c>
@@ -5056,7 +5083,7 @@
         <v>2.252283334204E-2</v>
       </c>
     </row>
-    <row r="150" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="24">
         <v>40798</v>
       </c>
@@ -5085,7 +5112,7 @@
         <v>2.2613975784474501E-2</v>
       </c>
     </row>
-    <row r="151" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="24">
         <v>40797</v>
       </c>
@@ -5114,7 +5141,7 @@
         <v>2.2705118226908998E-2</v>
       </c>
     </row>
-    <row r="152" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="24">
         <v>40796</v>
       </c>
@@ -5143,7 +5170,7 @@
         <v>2.27962606693436E-2</v>
       </c>
     </row>
-    <row r="153" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="24">
         <v>40795</v>
       </c>
@@ -5172,7 +5199,7 @@
         <v>2.2887403111778101E-2</v>
       </c>
     </row>
-    <row r="154" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="24">
         <v>40794</v>
       </c>
@@ -5201,7 +5228,7 @@
         <v>2.2978545554212599E-2</v>
       </c>
     </row>
-    <row r="155" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="24">
         <v>40793</v>
       </c>
@@ -5230,7 +5257,7 @@
         <v>2.30696879966471E-2</v>
       </c>
     </row>
-    <row r="156" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="24">
         <v>40792</v>
       </c>
@@ -5259,7 +5286,7 @@
         <v>2.3160830439081698E-2</v>
       </c>
     </row>
-    <row r="157" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="24">
         <v>40791</v>
       </c>
@@ -5288,7 +5315,7 @@
         <v>2.32519728815162E-2</v>
       </c>
     </row>
-    <row r="158" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="24">
         <v>40790</v>
       </c>
@@ -5317,7 +5344,7 @@
         <v>2.3343115323950701E-2</v>
       </c>
     </row>
-    <row r="159" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="24">
         <v>40789</v>
       </c>
@@ -5346,7 +5373,7 @@
         <v>2.3434257766385198E-2</v>
       </c>
     </row>
-    <row r="160" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="24">
         <v>40788</v>
       </c>
@@ -5375,7 +5402,7 @@
         <v>2.35254002088197E-2</v>
       </c>
     </row>
-    <row r="161" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="24">
         <v>40787</v>
       </c>
@@ -5404,7 +5431,7 @@
         <v>2.3616542651254301E-2</v>
       </c>
     </row>
-    <row r="162" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="24">
         <v>40786</v>
       </c>
@@ -5433,7 +5460,7 @@
         <v>2.36874489633595E-2</v>
       </c>
     </row>
-    <row r="163" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="24">
         <v>40785</v>
       </c>
@@ -5462,7 +5489,7 @@
         <v>2.3755143191285501E-2</v>
       </c>
     </row>
-    <row r="164" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="24">
         <v>40784</v>
       </c>
@@ -5491,7 +5518,7 @@
         <v>2.3822837419211401E-2</v>
       </c>
     </row>
-    <row r="165" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="24">
         <v>40783</v>
       </c>
@@ -5520,7 +5547,7 @@
         <v>2.3890531647137399E-2</v>
       </c>
     </row>
-    <row r="166" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="24">
         <v>40782</v>
       </c>
@@ -5549,7 +5576,7 @@
         <v>2.39582258750634E-2</v>
       </c>
     </row>
-    <row r="167" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="24">
         <v>40781</v>
       </c>
@@ -5578,7 +5605,7 @@
         <v>2.40259201029893E-2</v>
       </c>
     </row>
-    <row r="168" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="24">
         <v>40780</v>
       </c>
@@ -5607,7 +5634,7 @@
         <v>2.4093614330915301E-2</v>
       </c>
     </row>
-    <row r="169" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="24">
         <v>40779</v>
       </c>
@@ -5636,7 +5663,7 @@
         <v>2.4161308558841299E-2</v>
       </c>
     </row>
-    <row r="170" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="24">
         <v>40778</v>
       </c>
@@ -5665,7 +5692,7 @@
         <v>2.4229002786767199E-2</v>
       </c>
     </row>
-    <row r="171" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="24">
         <v>40777</v>
       </c>
@@ -5694,7 +5721,7 @@
         <v>2.4296697014693201E-2</v>
       </c>
     </row>
-    <row r="172" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="24">
         <v>40776</v>
       </c>
@@ -5723,7 +5750,7 @@
         <v>2.4364391242619202E-2</v>
       </c>
     </row>
-    <row r="173" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="24">
         <v>40775</v>
       </c>
@@ -5752,7 +5779,7 @@
         <v>2.4432085470545099E-2</v>
       </c>
     </row>
-    <row r="174" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="24">
         <v>40774</v>
       </c>
@@ -5781,7 +5808,7 @@
         <v>2.44997796984711E-2</v>
       </c>
     </row>
-    <row r="175" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="24">
         <v>40773</v>
       </c>
@@ -5810,7 +5837,7 @@
         <v>2.4567473926397101E-2</v>
       </c>
     </row>
-    <row r="176" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="24">
         <v>40772</v>
       </c>
@@ -5839,7 +5866,7 @@
         <v>2.4635168154323001E-2</v>
       </c>
     </row>
-    <row r="177" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="24">
         <v>40771</v>
       </c>
@@ -5868,7 +5895,7 @@
         <v>2.4702862382248999E-2</v>
       </c>
     </row>
-    <row r="178" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="24">
         <v>40770</v>
       </c>
@@ -5897,7 +5924,7 @@
         <v>2.4770556610175E-2</v>
       </c>
     </row>
-    <row r="179" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="24">
         <v>40769</v>
       </c>
@@ -5926,7 +5953,7 @@
         <v>2.48382508381009E-2</v>
       </c>
     </row>
-    <row r="180" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="24">
         <v>40768</v>
       </c>
@@ -5955,7 +5982,7 @@
         <v>2.4905945066026901E-2</v>
       </c>
     </row>
-    <row r="181" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="24">
         <v>40767</v>
       </c>
@@ -5984,7 +6011,7 @@
         <v>2.4973639293952899E-2</v>
       </c>
     </row>
-    <row r="182" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="24">
         <v>40766</v>
       </c>
@@ -6013,7 +6040,7 @@
         <v>2.5035748036402201E-2</v>
       </c>
     </row>
-    <row r="183" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="24">
         <v>40765</v>
       </c>
@@ -6042,7 +6069,7 @@
         <v>2.50969701938553E-2</v>
       </c>
     </row>
-    <row r="184" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="24">
         <v>40764</v>
       </c>
@@ -6071,7 +6098,7 @@
         <v>2.5158192351308301E-2</v>
       </c>
     </row>
-    <row r="185" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="24">
         <v>40763</v>
       </c>
@@ -6100,7 +6127,7 @@
         <v>2.52194145087614E-2</v>
       </c>
     </row>
-    <row r="186" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="24">
         <v>40762</v>
       </c>
@@ -6129,7 +6156,7 @@
         <v>2.5280636666214499E-2</v>
       </c>
     </row>
-    <row r="187" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="24">
         <v>40761</v>
       </c>
@@ -6158,7 +6185,7 @@
         <v>2.5341858823667501E-2</v>
       </c>
     </row>
-    <row r="188" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="24">
         <v>40760</v>
       </c>
@@ -6187,7 +6214,7 @@
         <v>2.5403080981120599E-2</v>
       </c>
     </row>
-    <row r="189" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="24">
         <v>40759</v>
       </c>
@@ -6216,7 +6243,7 @@
         <v>2.5464303138573601E-2</v>
       </c>
     </row>
-    <row r="190" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="24">
         <v>40758</v>
       </c>
@@ -6245,7 +6272,7 @@
         <v>2.55255252960267E-2</v>
       </c>
     </row>
-    <row r="191" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="24">
         <v>40757</v>
       </c>
@@ -6274,7 +6301,7 @@
         <v>2.5586747453479702E-2</v>
       </c>
     </row>
-    <row r="192" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="24">
         <v>40756</v>
       </c>
@@ -6303,7 +6330,7 @@
         <v>2.5647969610932801E-2</v>
       </c>
     </row>
-    <row r="193" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="24">
         <v>40755</v>
       </c>
@@ -6332,7 +6359,7 @@
         <v>2.5709191768385899E-2</v>
       </c>
     </row>
-    <row r="194" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="24">
         <v>40754</v>
       </c>
@@ -6361,7 +6388,7 @@
         <v>2.5770413925838901E-2</v>
       </c>
     </row>
-    <row r="195" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="24">
         <v>40753</v>
       </c>
@@ -6390,7 +6417,7 @@
         <v>2.5831636083292E-2</v>
       </c>
     </row>
-    <row r="196" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="24">
         <v>40752</v>
       </c>
@@ -6419,7 +6446,7 @@
         <v>2.5892858240745002E-2</v>
       </c>
     </row>
-    <row r="197" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="24">
         <v>40751</v>
       </c>
@@ -6448,7 +6475,7 @@
         <v>2.59540803981981E-2</v>
       </c>
     </row>
-    <row r="198" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="24">
         <v>40750</v>
       </c>
@@ -6477,7 +6504,7 @@
         <v>2.6015302555651199E-2</v>
       </c>
     </row>
-    <row r="199" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="24">
         <v>40749</v>
       </c>
@@ -6506,7 +6533,7 @@
         <v>2.6076524713104201E-2</v>
       </c>
     </row>
-    <row r="200" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="24">
         <v>40748</v>
       </c>
@@ -6535,7 +6562,7 @@
         <v>2.61377468705573E-2</v>
       </c>
     </row>
-    <row r="201" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="24">
         <v>40747</v>
       </c>
@@ -6564,7 +6591,7 @@
         <v>2.6198969028010301E-2</v>
       </c>
     </row>
-    <row r="202" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="24">
         <v>40746</v>
       </c>
@@ -6593,7 +6620,7 @@
         <v>2.6277768937171399E-2</v>
       </c>
     </row>
-    <row r="203" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="24">
         <v>40745</v>
       </c>
@@ -6622,7 +6649,7 @@
         <v>2.6362321565073201E-2</v>
       </c>
     </row>
-    <row r="204" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="24">
         <v>40744</v>
       </c>
@@ -6651,7 +6678,7 @@
         <v>2.6446874192974999E-2</v>
       </c>
     </row>
-    <row r="205" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="24">
         <v>40743</v>
       </c>
@@ -6680,7 +6707,7 @@
         <v>2.6531426820876801E-2</v>
       </c>
     </row>
-    <row r="206" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="24">
         <v>40742</v>
       </c>
@@ -6709,7 +6736,7 @@
         <v>2.66159794487787E-2</v>
       </c>
     </row>
-    <row r="207" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="24">
         <v>40741</v>
       </c>
@@ -6738,7 +6765,7 @@
         <v>2.6700532076680501E-2</v>
       </c>
     </row>
-    <row r="208" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="24">
         <v>40740</v>
       </c>
@@ -6767,7 +6794,7 @@
         <v>2.6785084704582299E-2</v>
       </c>
     </row>
-    <row r="209" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="24">
         <v>40739</v>
       </c>
@@ -6796,7 +6823,7 @@
         <v>2.6869637332484101E-2</v>
       </c>
     </row>
-    <row r="210" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="24">
         <v>40738</v>
       </c>
@@ -6825,7 +6852,7 @@
         <v>2.6954189960386E-2</v>
       </c>
     </row>
-    <row r="211" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="24">
         <v>40737</v>
       </c>
@@ -6854,7 +6881,7 @@
         <v>2.7038742588287801E-2</v>
       </c>
     </row>
-    <row r="212" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="24">
         <v>40736</v>
       </c>
@@ -6883,7 +6910,7 @@
         <v>2.71232952161896E-2</v>
       </c>
     </row>
-    <row r="213" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="24">
         <v>40735</v>
       </c>
@@ -6912,7 +6939,7 @@
         <v>2.7207847844091498E-2</v>
       </c>
     </row>
-    <row r="214" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="24">
         <v>40734</v>
       </c>
@@ -6941,7 +6968,7 @@
         <v>2.72924004719933E-2</v>
       </c>
     </row>
-    <row r="215" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="24">
         <v>40733</v>
       </c>
@@ -6970,7 +6997,7 @@
         <v>2.7376953099895102E-2</v>
       </c>
     </row>
-    <row r="216" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B216" s="24">
         <v>40732</v>
       </c>
@@ -6999,7 +7026,7 @@
         <v>2.7461505727797E-2</v>
       </c>
     </row>
-    <row r="217" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="24">
         <v>40731</v>
       </c>
@@ -7028,7 +7055,7 @@
         <v>2.7546058355698799E-2</v>
       </c>
     </row>
-    <row r="218" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="24">
         <v>40730</v>
       </c>
@@ -7057,7 +7084,7 @@
         <v>2.76306109836006E-2</v>
       </c>
     </row>
-    <row r="219" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B219" s="24">
         <v>40729</v>
       </c>
@@ -7086,7 +7113,7 @@
         <v>2.7715163611502398E-2</v>
       </c>
     </row>
-    <row r="220" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B220" s="24">
         <v>40728</v>
       </c>
@@ -7115,7 +7142,7 @@
         <v>2.7799716239404301E-2</v>
       </c>
     </row>
-    <row r="221" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B221" s="24">
         <v>40727</v>
       </c>
@@ -7144,7 +7171,7 @@
         <v>2.7884268867306099E-2</v>
       </c>
     </row>
-    <row r="222" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B222" s="24">
         <v>40726</v>
       </c>
@@ -7173,7 +7200,7 @@
         <v>2.7940298038756198E-2</v>
       </c>
     </row>
-    <row r="223" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223" s="24">
         <v>40725</v>
       </c>
@@ -7202,7 +7229,7 @@
         <v>2.7989558932404301E-2</v>
       </c>
     </row>
-    <row r="224" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224" s="24">
         <v>40724</v>
       </c>
@@ -7231,7 +7258,7 @@
         <v>2.8038819826052299E-2</v>
       </c>
     </row>
-    <row r="225" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B225" s="24">
         <v>40723</v>
       </c>
@@ -7260,7 +7287,7 @@
         <v>2.8088080719700301E-2</v>
       </c>
     </row>
-    <row r="226" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226" s="24">
         <v>40722</v>
       </c>
@@ -7289,7 +7316,7 @@
         <v>2.81373416133484E-2</v>
       </c>
     </row>
-    <row r="227" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="24">
         <v>40721</v>
       </c>
@@ -7318,7 +7345,7 @@
         <v>2.8186602506996401E-2</v>
       </c>
     </row>
-    <row r="228" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B228" s="24">
         <v>40720</v>
       </c>
@@ -7347,7 +7374,7 @@
         <v>2.82358634006445E-2</v>
       </c>
     </row>
-    <row r="229" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B229" s="24">
         <v>40719</v>
       </c>
@@ -7376,7 +7403,7 @@
         <v>2.8285124294292498E-2</v>
       </c>
     </row>
-    <row r="230" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B230" s="24">
         <v>40718</v>
       </c>
@@ -7405,7 +7432,7 @@
         <v>2.83343851879405E-2</v>
       </c>
     </row>
-    <row r="231" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B231" s="24">
         <v>40717</v>
       </c>
@@ -7434,7 +7461,7 @@
         <v>2.8383646081588599E-2</v>
       </c>
     </row>
-    <row r="232" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B232" s="24">
         <v>40716</v>
       </c>
@@ -7463,7 +7490,7 @@
         <v>2.8432906975236601E-2</v>
       </c>
     </row>
-    <row r="233" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B233" s="24">
         <v>40715</v>
       </c>
@@ -7492,7 +7519,7 @@
         <v>2.8482167868884599E-2</v>
       </c>
     </row>
-    <row r="234" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B234" s="24">
         <v>40714</v>
       </c>
@@ -7521,7 +7548,7 @@
         <v>2.8531428762532701E-2</v>
       </c>
     </row>
-    <row r="235" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B235" s="24">
         <v>40713</v>
       </c>
@@ -7550,7 +7577,7 @@
         <v>2.8580689656180699E-2</v>
       </c>
     </row>
-    <row r="236" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B236" s="24">
         <v>40712</v>
       </c>
@@ -7579,7 +7606,7 @@
         <v>2.8629950549828701E-2</v>
       </c>
     </row>
-    <row r="237" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B237" s="24">
         <v>40711</v>
       </c>
@@ -7608,7 +7635,7 @@
         <v>2.86792114434768E-2</v>
       </c>
     </row>
-    <row r="238" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B238" s="24">
         <v>40710</v>
       </c>
@@ -7637,7 +7664,7 @@
         <v>2.8728472337124802E-2</v>
       </c>
     </row>
-    <row r="239" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B239" s="24">
         <v>40709</v>
       </c>
@@ -7666,7 +7693,7 @@
         <v>2.8777733230772901E-2</v>
       </c>
     </row>
-    <row r="240" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B240" s="24">
         <v>40708</v>
       </c>
@@ -7695,7 +7722,7 @@
         <v>2.8826994124420899E-2</v>
       </c>
     </row>
-    <row r="241" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B241" s="24">
         <v>40707</v>
       </c>
@@ -7724,7 +7751,7 @@
         <v>2.8876255018068901E-2</v>
       </c>
     </row>
-    <row r="242" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="24">
         <v>40706</v>
       </c>
@@ -7753,7 +7780,7 @@
         <v>2.8925515911716999E-2</v>
       </c>
     </row>
-    <row r="243" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="24">
         <v>40705</v>
       </c>
@@ -7782,7 +7809,7 @@
         <v>2.8974776805365001E-2</v>
       </c>
     </row>
-    <row r="244" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="24">
         <v>40704</v>
       </c>
@@ -7811,7 +7838,7 @@
         <v>2.9024037699012999E-2</v>
       </c>
     </row>
-    <row r="245" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B245" s="24">
         <v>40703</v>
       </c>
@@ -7840,7 +7867,7 @@
         <v>2.9073298592661102E-2</v>
       </c>
     </row>
-    <row r="246" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B246" s="24">
         <v>40702</v>
       </c>
@@ -7869,7 +7896,7 @@
         <v>2.91225594863091E-2</v>
       </c>
     </row>
-    <row r="247" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="24">
         <v>40701</v>
       </c>
@@ -7898,7 +7925,7 @@
         <v>2.9171820379957199E-2</v>
       </c>
     </row>
-    <row r="248" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B248" s="24">
         <v>40700</v>
       </c>
@@ -7927,7 +7954,7 @@
         <v>2.92210812736052E-2</v>
       </c>
     </row>
-    <row r="249" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B249" s="24">
         <v>40699</v>
       </c>
@@ -7956,7 +7983,7 @@
         <v>2.9270342167253199E-2</v>
       </c>
     </row>
-    <row r="250" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B250" s="24">
         <v>40698</v>
       </c>
@@ -7985,7 +8012,7 @@
         <v>2.9319603060901301E-2</v>
       </c>
     </row>
-    <row r="251" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B251" s="24">
         <v>40697</v>
       </c>
@@ -8014,7 +8041,7 @@
         <v>2.9368863954549299E-2</v>
       </c>
     </row>
-    <row r="252" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B252" s="24">
         <v>40696</v>
       </c>
@@ -8043,7 +8070,7 @@
         <v>2.9418124848197301E-2</v>
       </c>
     </row>
-    <row r="253" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B253" s="24">
         <v>40695</v>
       </c>
@@ -8072,7 +8099,7 @@
         <v>2.94673857418454E-2</v>
       </c>
     </row>
-    <row r="254" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B254" s="24">
         <v>40694</v>
       </c>
@@ -8101,7 +8128,7 @@
         <v>2.9516646635493402E-2</v>
       </c>
     </row>
-    <row r="255" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B255" s="24">
         <v>40693</v>
       </c>
@@ -8130,7 +8157,7 @@
         <v>2.95659075291414E-2</v>
       </c>
     </row>
-    <row r="256" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B256" s="24">
         <v>40692</v>
       </c>
@@ -8159,7 +8186,7 @@
         <v>2.9615168422789499E-2</v>
       </c>
     </row>
-    <row r="257" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B257" s="24">
         <v>40691</v>
       </c>
@@ -8188,7 +8215,7 @@
         <v>2.96644293164375E-2</v>
       </c>
     </row>
-    <row r="258" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B258" s="24">
         <v>40690</v>
       </c>
@@ -8217,7 +8244,7 @@
         <v>2.9713690210085599E-2</v>
       </c>
     </row>
-    <row r="259" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B259" s="24">
         <v>40689</v>
       </c>
@@ -8246,7 +8273,7 @@
         <v>2.9762951103733601E-2</v>
       </c>
     </row>
-    <row r="260" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B260" s="24">
         <v>40688</v>
       </c>
@@ -8275,7 +8302,7 @@
         <v>2.9812211997381599E-2</v>
       </c>
     </row>
-    <row r="261" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B261" s="24">
         <v>40687</v>
       </c>
@@ -8304,7 +8331,7 @@
         <v>2.9861472891029701E-2</v>
       </c>
     </row>
-    <row r="262" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B262" s="24">
         <v>40686</v>
       </c>
@@ -8333,7 +8360,7 @@
         <v>2.9832712380565601E-2</v>
       </c>
     </row>
-    <row r="263" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B263" s="24">
         <v>40685</v>
       </c>
@@ -8362,7 +8389,7 @@
         <v>2.9785438316583299E-2</v>
       </c>
     </row>
-    <row r="264" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B264" s="24">
         <v>40684</v>
       </c>
@@ -8391,7 +8418,7 @@
         <v>2.9738164252601101E-2</v>
       </c>
     </row>
-    <row r="265" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B265" s="24">
         <v>40683</v>
       </c>
@@ -8420,7 +8447,7 @@
         <v>2.9690890188618799E-2</v>
       </c>
     </row>
-    <row r="266" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B266" s="24">
         <v>40682</v>
       </c>
@@ -8449,7 +8476,7 @@
         <v>2.96436161246365E-2</v>
       </c>
     </row>
-    <row r="267" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B267" s="24">
         <v>40681</v>
       </c>
@@ -8478,7 +8505,7 @@
         <v>2.9596342060654299E-2</v>
       </c>
     </row>
-    <row r="268" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B268" s="24">
         <v>40680</v>
       </c>
@@ -8507,7 +8534,7 @@
         <v>2.9549067996672E-2</v>
       </c>
     </row>
-    <row r="269" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B269" s="24">
         <v>40679</v>
       </c>
@@ -8536,7 +8563,7 @@
         <v>2.9501793932689799E-2</v>
       </c>
     </row>
-    <row r="270" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B270" s="24">
         <v>40678</v>
       </c>
@@ -8565,7 +8592,7 @@
         <v>2.94545198687075E-2</v>
       </c>
     </row>
-    <row r="271" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B271" s="24">
         <v>40677</v>
       </c>
@@ -8594,7 +8621,7 @@
         <v>2.9407245804725299E-2</v>
       </c>
     </row>
-    <row r="272" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B272" s="24">
         <v>40676</v>
       </c>
@@ -8623,7 +8650,7 @@
         <v>2.9359971740743E-2</v>
       </c>
     </row>
-    <row r="273" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B273" s="24">
         <v>40675</v>
       </c>
@@ -8652,7 +8679,7 @@
         <v>2.9312697676760799E-2</v>
       </c>
     </row>
-    <row r="274" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B274" s="24">
         <v>40674</v>
       </c>
@@ -8681,7 +8708,7 @@
         <v>2.92654236127785E-2</v>
       </c>
     </row>
-    <row r="275" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B275" s="24">
         <v>40673</v>
       </c>
@@ -8710,7 +8737,7 @@
         <v>2.9218149548796299E-2</v>
       </c>
     </row>
-    <row r="276" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B276" s="24">
         <v>40672</v>
       </c>
@@ -8739,7 +8766,7 @@
         <v>2.9170875484814E-2</v>
       </c>
     </row>
-    <row r="277" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B277" s="24">
         <v>40671</v>
       </c>
@@ -8768,7 +8795,7 @@
         <v>2.9123601420831698E-2</v>
       </c>
     </row>
-    <row r="278" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B278" s="24">
         <v>40670</v>
       </c>
@@ -8797,7 +8824,7 @@
         <v>2.90763273568495E-2</v>
       </c>
     </row>
-    <row r="279" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B279" s="24">
         <v>40669</v>
       </c>
@@ -8826,7 +8853,7 @@
         <v>2.9029053292867198E-2</v>
       </c>
     </row>
-    <row r="280" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B280" s="24">
         <v>40668</v>
       </c>
@@ -8855,7 +8882,7 @@
         <v>2.8981779228885E-2</v>
       </c>
     </row>
-    <row r="281" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B281" s="24">
         <v>40667</v>
       </c>
@@ -8884,7 +8911,7 @@
         <v>2.8934505164902698E-2</v>
       </c>
     </row>
-    <row r="282" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B282" s="24">
         <v>40666</v>
       </c>
@@ -8913,7 +8940,7 @@
         <v>2.88872311009205E-2</v>
       </c>
     </row>
-    <row r="283" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B283" s="24">
         <v>40665</v>
       </c>
@@ -8942,7 +8969,7 @@
         <v>2.8839957036938198E-2</v>
       </c>
     </row>
-    <row r="284" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B284" s="24">
         <v>40664</v>
       </c>
@@ -8971,7 +8998,7 @@
         <v>2.8792682972956E-2</v>
       </c>
     </row>
-    <row r="285" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B285" s="24">
         <v>40663</v>
       </c>
@@ -9000,7 +9027,7 @@
         <v>2.8745408908973698E-2</v>
       </c>
     </row>
-    <row r="286" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B286" s="24">
         <v>40662</v>
       </c>
@@ -9029,7 +9056,7 @@
         <v>2.8698134844991501E-2</v>
       </c>
     </row>
-    <row r="287" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B287" s="24">
         <v>40661</v>
       </c>
@@ -9058,7 +9085,7 @@
         <v>2.8650860781009101E-2</v>
       </c>
     </row>
-    <row r="288" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B288" s="24">
         <v>40660</v>
       </c>
@@ -9087,7 +9114,7 @@
         <v>2.86035867170269E-2</v>
       </c>
     </row>
-    <row r="289" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B289" s="24">
         <v>40659</v>
       </c>
@@ -9116,7 +9143,7 @@
         <v>2.8556312653044601E-2</v>
       </c>
     </row>
-    <row r="290" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B290" s="24">
         <v>40658</v>
       </c>
@@ -9145,7 +9172,7 @@
         <v>2.8509038589062299E-2</v>
       </c>
     </row>
-    <row r="291" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B291" s="24">
         <v>40657</v>
       </c>
@@ -9174,7 +9201,7 @@
         <v>2.8461764525080101E-2</v>
       </c>
     </row>
-    <row r="292" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B292" s="24">
         <v>40656</v>
       </c>
@@ -9203,7 +9230,7 @@
         <v>2.8414490461097799E-2</v>
       </c>
     </row>
-    <row r="293" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B293" s="24">
         <v>40655</v>
       </c>
@@ -9232,7 +9259,7 @@
         <v>2.8367216397115601E-2</v>
       </c>
     </row>
-    <row r="294" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B294" s="24">
         <v>40654</v>
       </c>
@@ -9261,7 +9288,7 @@
         <v>2.8319942333133299E-2</v>
       </c>
     </row>
-    <row r="295" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B295" s="24">
         <v>40653</v>
       </c>
@@ -9290,7 +9317,7 @@
         <v>2.8272668269151102E-2</v>
       </c>
     </row>
-    <row r="296" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B296" s="24">
         <v>40652</v>
       </c>
@@ -9319,7 +9346,7 @@
         <v>2.8225394205168799E-2</v>
       </c>
     </row>
-    <row r="297" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B297" s="24">
         <v>40651</v>
       </c>
@@ -9348,7 +9375,7 @@
         <v>2.8178120141186602E-2</v>
       </c>
     </row>
-    <row r="298" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B298" s="24">
         <v>40650</v>
       </c>
@@ -9377,7 +9404,7 @@
         <v>2.81308460772043E-2</v>
       </c>
     </row>
-    <row r="299" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B299" s="24">
         <v>40649</v>
       </c>
@@ -9406,7 +9433,7 @@
         <v>2.8083572013222102E-2</v>
       </c>
     </row>
-    <row r="300" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B300" s="24">
         <v>40648</v>
       </c>
@@ -9435,7 +9462,7 @@
         <v>2.80362979492398E-2</v>
       </c>
     </row>
-    <row r="301" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B301" s="24">
         <v>40647</v>
       </c>
@@ -9464,7 +9491,7 @@
         <v>2.7989023885257602E-2</v>
       </c>
     </row>
-    <row r="302" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B302" s="24">
         <v>40646</v>
       </c>
@@ -9493,7 +9520,7 @@
         <v>2.79417498212753E-2</v>
       </c>
     </row>
-    <row r="303" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B303" s="24">
         <v>40645</v>
       </c>
@@ -9522,7 +9549,7 @@
         <v>2.7894475757293001E-2</v>
       </c>
     </row>
-    <row r="304" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B304" s="24">
         <v>40644</v>
       </c>
@@ -9551,7 +9578,7 @@
         <v>2.78472016933108E-2</v>
       </c>
     </row>
-    <row r="305" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B305" s="24">
         <v>40643</v>
       </c>
@@ -9580,7 +9607,7 @@
         <v>2.7799927629328501E-2</v>
       </c>
     </row>
-    <row r="306" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B306" s="24">
         <v>40642</v>
       </c>
@@ -9609,7 +9636,7 @@
         <v>2.77526535653463E-2</v>
       </c>
     </row>
-    <row r="307" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B307" s="24">
         <v>40641</v>
       </c>
@@ -9638,7 +9665,7 @@
         <v>2.7705379501364001E-2</v>
       </c>
     </row>
-    <row r="308" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B308" s="24">
         <v>40640</v>
       </c>
@@ -9667,7 +9694,7 @@
         <v>2.76581054373818E-2</v>
       </c>
     </row>
-    <row r="309" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B309" s="24">
         <v>40639</v>
       </c>
@@ -9696,7 +9723,7 @@
         <v>2.7610831373399501E-2</v>
       </c>
     </row>
-    <row r="310" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B310" s="24">
         <v>40638</v>
       </c>
@@ -9725,7 +9752,7 @@
         <v>2.75635573094173E-2</v>
       </c>
     </row>
-    <row r="311" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B311" s="24">
         <v>40637</v>
       </c>
@@ -9754,7 +9781,7 @@
         <v>2.7516283245435001E-2</v>
       </c>
     </row>
-    <row r="312" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B312" s="24">
         <v>40636</v>
       </c>
@@ -9783,7 +9810,7 @@
         <v>2.74690091814528E-2</v>
       </c>
     </row>
-    <row r="313" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B313" s="24">
         <v>40635</v>
       </c>
@@ -9812,7 +9839,7 @@
         <v>2.7421735117470501E-2</v>
       </c>
     </row>
-    <row r="314" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B314" s="24">
         <v>40634</v>
       </c>
@@ -9841,7 +9868,7 @@
         <v>2.7374461053488199E-2</v>
       </c>
     </row>
-    <row r="315" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B315" s="24">
         <v>40633</v>
       </c>
@@ -9870,7 +9897,7 @@
         <v>2.7327186989506001E-2</v>
       </c>
     </row>
-    <row r="316" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B316" s="24">
         <v>40632</v>
       </c>
@@ -9899,7 +9926,7 @@
         <v>2.7279912925523699E-2</v>
       </c>
     </row>
-    <row r="317" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B317" s="24">
         <v>40631</v>
       </c>
@@ -9928,7 +9955,7 @@
         <v>2.7232638861541501E-2</v>
       </c>
     </row>
-    <row r="318" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B318" s="24">
         <v>40630</v>
       </c>
@@ -9957,7 +9984,7 @@
         <v>2.7185364797559199E-2</v>
       </c>
     </row>
-    <row r="319" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B319" s="24">
         <v>40629</v>
       </c>
@@ -9986,7 +10013,7 @@
         <v>2.7138090733577001E-2</v>
       </c>
     </row>
-    <row r="320" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B320" s="24">
         <v>40628</v>
       </c>
@@ -10015,7 +10042,7 @@
         <v>2.7090816669594699E-2</v>
       </c>
     </row>
-    <row r="321" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B321" s="24">
         <v>40627</v>
       </c>
@@ -10044,7 +10071,7 @@
         <v>2.7043542605612501E-2</v>
       </c>
     </row>
-    <row r="322" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B322" s="24">
         <v>40626</v>
       </c>
@@ -10073,7 +10100,7 @@
         <v>2.6990304408710801E-2</v>
       </c>
     </row>
-    <row r="323" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B323" s="24">
         <v>40625</v>
       </c>
@@ -10102,7 +10129,7 @@
         <v>2.6934493448589E-2</v>
       </c>
     </row>
-    <row r="324" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B324" s="24">
         <v>40624</v>
       </c>
@@ -10131,7 +10158,7 @@
         <v>2.6878682488467202E-2</v>
       </c>
     </row>
-    <row r="325" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B325" s="24">
         <v>40623</v>
       </c>
@@ -10160,7 +10187,7 @@
         <v>2.6822871528345501E-2</v>
       </c>
     </row>
-    <row r="326" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B326" s="24">
         <v>40622</v>
       </c>
@@ -10189,7 +10216,7 @@
         <v>2.67670605682237E-2</v>
       </c>
     </row>
-    <row r="327" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B327" s="24">
         <v>40621</v>
       </c>
@@ -10218,7 +10245,7 @@
         <v>2.6711249608101902E-2</v>
       </c>
     </row>
-    <row r="328" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B328" s="24">
         <v>40620</v>
       </c>
@@ -10247,7 +10274,7 @@
         <v>2.66554386479801E-2</v>
       </c>
     </row>
-    <row r="329" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B329" s="24">
         <v>40619</v>
       </c>
@@ -10276,7 +10303,7 @@
         <v>2.6599627687858399E-2</v>
       </c>
     </row>
-    <row r="330" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B330" s="24">
         <v>40618</v>
       </c>
@@ -10305,7 +10332,7 @@
         <v>2.6543816727736601E-2</v>
       </c>
     </row>
-    <row r="331" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B331" s="24">
         <v>40617</v>
       </c>
@@ -10334,7 +10361,7 @@
         <v>2.64880057676148E-2</v>
       </c>
     </row>
-    <row r="332" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B332" s="24">
         <v>40616</v>
       </c>
@@ -10363,7 +10390,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="333" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B333" s="24">
         <v>40615</v>
       </c>
@@ -10392,7 +10419,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="334" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B334" s="24">
         <v>40614</v>
       </c>
@@ -10421,7 +10448,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="335" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B335" s="24">
         <v>40613</v>
       </c>
@@ -10450,7 +10477,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="336" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B336" s="24">
         <v>40612</v>
       </c>
@@ -10479,7 +10506,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="337" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B337" s="24">
         <v>40611</v>
       </c>
@@ -10508,7 +10535,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="338" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B338" s="24">
         <v>40610</v>
       </c>
@@ -10537,7 +10564,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="339" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B339" s="24">
         <v>40609</v>
       </c>
@@ -10566,7 +10593,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="340" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B340" s="24">
         <v>40608</v>
       </c>
@@ -10595,7 +10622,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="341" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B341" s="24">
         <v>40607</v>
       </c>
@@ -10624,7 +10651,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="342" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B342" s="24">
         <v>40606</v>
       </c>
@@ -10653,7 +10680,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="343" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B343" s="24">
         <v>40605</v>
       </c>
@@ -10682,7 +10709,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="344" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B344" s="24">
         <v>40604</v>
       </c>
@@ -10711,7 +10738,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="345" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B345" s="24">
         <v>40603</v>
       </c>
@@ -10740,7 +10767,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="346" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B346" s="24">
         <v>40602</v>
       </c>
@@ -10769,7 +10796,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="347" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B347" s="24">
         <v>40601</v>
       </c>
@@ -10798,7 +10825,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="348" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B348" s="24">
         <v>40600</v>
       </c>
@@ -10827,7 +10854,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="349" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B349" s="24">
         <v>40599</v>
       </c>
@@ -10856,7 +10883,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="350" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B350" s="24">
         <v>40598</v>
       </c>
@@ -10885,7 +10912,7 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="351" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B351" s="24">
         <v>40597</v>
       </c>
@@ -10914,6 +10941,12 @@
         <v>2.6499999999999999E-2</v>
       </c>
     </row>
+    <row r="352" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1048479" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1048480" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1048481" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11014,7 +11047,7 @@
     <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
@@ -11024,18 +11057,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AMK60"/>
+  <dimension ref="A2:AMK85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" style="27"/>
-    <col min="2" max="7" width="11.54296875" style="16"/>
-    <col min="8" max="8" width="11.54296875" style="28"/>
-    <col min="9" max="12" width="11.54296875" style="16"/>
-    <col min="13" max="13" width="11.54296875" style="28"/>
-    <col min="14" max="1025" width="11.54296875" style="16"/>
+    <col min="1" max="1" width="5.109375" style="27" customWidth="1"/>
+    <col min="2" max="7" width="11.5546875" style="16"/>
+    <col min="8" max="8" width="11.5546875" style="28"/>
+    <col min="9" max="12" width="11.5546875" style="16"/>
+    <col min="13" max="13" width="11.5546875" style="28"/>
+    <col min="14" max="1025" width="11.5546875" style="16"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -11095,9 +11128,9 @@
         <v>57</v>
       </c>
       <c r="E7" s="12" t="str">
-        <f>[1]!obMake("baseDate-cap",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",F7))</f>
+        <f>[1]!obMake("baseDate-cap","LocalDate",F7)</f>
         <v>baseDate-cap 
-[13070]</v>
+[6024]</v>
       </c>
       <c r="F7" s="17">
         <v>40918</v>
@@ -11111,14 +11144,14 @@
       <c r="N7" s="12" t="str">
         <f>'Curves Definition'!F8</f>
         <v>modelWithForwardAndDiscountingCurves 
-[13240]</v>
+[6435]</v>
       </c>
     </row>
     <row r="8" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="str">
-        <f>[1]!obMake("referenceDate "&amp;COLUMN(),obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",C8))</f>
+        <f>[1]!obMake("referenceDate "&amp;COLUMN(),"LocalDate",C8)</f>
         <v>referenceDate 2 
-[12969]</v>
+[6076]</v>
       </c>
       <c r="C8" s="17">
         <v>40918</v>
@@ -11126,7 +11159,7 @@
       <c r="E8" s="12" t="str">
         <f>[1]!obMake("shortPeriod-cap","String",F8)</f>
         <v>shortPeriod-cap 
-[12885]</v>
+[6014]</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>59</v>
@@ -11148,12 +11181,12 @@
       <c r="C9" s="12" t="str">
         <f>'Curves Definition'!F28</f>
         <v>forward-EUR-3M 
-[13179]</v>
+[6321]</v>
       </c>
       <c r="E9" s="12" t="str">
         <f>[1]!obMake("businessDayCal-cap",obLibs&amp;"net.finmath.time.businessdaycalendar."&amp;F9)</f>
         <v>businessDayCal-cap 
-[12985]</v>
+[6149]</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>39</v>
@@ -11167,9 +11200,9 @@
     </row>
     <row r="10" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="str">
-        <f>[1]!OBCALL("quotingConvention "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurfaceInterface$QuotingConvention","valueOf",[1]!obMake("","String",C10))</f>
+        <f>[1]!obCall("quotingConvention "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurface$QuotingConvention","valueOf",[1]!obMake("","String",C10))</f>
         <v>quotingConvention 2 
-[13009]</v>
+[6198]</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>56</v>
@@ -11181,9 +11214,9 @@
         <v>40920</v>
       </c>
       <c r="N10" s="12" t="str">
-        <f>[1]!OBCALL("modelWithVolSurface",N7,"addVolatilitySurface",B14)</f>
+        <f>[1]!obCall("modelWithVolSurface",N7,"addVolatilitySurface",B14)</f>
         <v>modelWithVolSurface 
-[13358]</v>
+[6441]</v>
       </c>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
@@ -11195,7 +11228,7 @@
       <c r="C11" s="12" t="str">
         <f>'Curves Definition'!B28</f>
         <v>curveObject-discount-EUR-OIS-curveDef 
-[13059]</v>
+[6189]</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>65</v>
@@ -11219,9 +11252,9 @@
         <v>68</v>
       </c>
       <c r="AC12" s="16" t="str">
-        <f>[1]!OBCALL("quotingConventionResult "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurfaceInterface$QuotingConvention","valueOf",[1]!obMake("","String",AC11))</f>
+        <f>[1]!obCall("quotingConventionResult "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurface$QuotingConvention","valueOf",[1]!obMake("","String",AC11))</f>
         <v>quotingConventionResult 29 
-[12989]</v>
+[6089]</v>
       </c>
     </row>
     <row r="13" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -11241,7 +11274,7 @@
       <c r="B14" s="22" t="str">
         <f>[1]!obMake("capletVolatility",obLibs&amp;"net.finmath.marketdata.model.volatilities.CapletVolatilities",[1]!obMake("","String",C7),B8,C9,[1]!obMake("","double[]",B34:B60),[1]!obMake("","double[]",C34:C60),[1]!obMake("","double[]",D34:D60),B10,C11)</f>
         <v>capletVolatility 
-[13357]</v>
+[6440]</v>
       </c>
       <c r="C14" s="12"/>
       <c r="E14" s="16" t="s">
@@ -11301,9 +11334,9 @@
         <v>0</v>
       </c>
       <c r="N15" s="19" t="str">
-        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!OBCALL("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",O15)),[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",P15)),[1]!obMake("","String",Q15),[1]!obMake("","String",R15),$E$8,[1]!obMake("","String",S15),$E$9,[1]!obMake("","int",T15),[1]!obMake("","int",U15)),[1]!obMake("","String",V15),[1]!obMake("","double",W15),[1]!obMake("","boolean",X15),[1]!obMake("","String",Y15),[1]!obMake("","String",Z15))</f>
+        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!obCall("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("","LocalDate",O15),[1]!obMake("","LocalDate",P15),[1]!obMake("","String",Q15),[1]!obMake("","String",R15),$E$8,[1]!obMake("","String",S15),$E$9,[1]!obMake("","int",T15),[1]!obMake("","int",U15)),[1]!obMake("","String",V15),[1]!obMake("","double",W15),[1]!obMake("","boolean",X15),[1]!obMake("","String",Y15),[1]!obMake("","String",Z15))</f>
         <v>cap-15 
-[13151]</v>
+[6164]</v>
       </c>
       <c r="O15" s="31">
         <v>40980</v>
@@ -11345,11 +11378,11 @@
         <v>capletVol</v>
       </c>
       <c r="AB15" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N15,"getValue",$N$10))</f>
+        <f>[1]!obGet([1]!obCall("",N15,"getValue",$N$10))</f>
         <v>8.2752528962869406E-5</v>
       </c>
       <c r="AC15" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N15,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
+        <f>[1]!obGet([1]!obCall("",N15,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
         <v>0.7</v>
       </c>
     </row>
@@ -11361,9 +11394,9 @@
         <v>0</v>
       </c>
       <c r="N16" s="19" t="str">
-        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!OBCALL("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",O16)),[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",P16)),[1]!obMake("","String",Q16),[1]!obMake("","String",R16),$E$8,[1]!obMake("","String",S16),$E$9,[1]!obMake("","int",T16),[1]!obMake("","int",U16)),[1]!obMake("","String",V16),[1]!obMake("","double",W16),[1]!obMake("","boolean",X16),[1]!obMake("","String",Y16),[1]!obMake("","String",Z16))</f>
+        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!obCall("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("","LocalDate",O16),[1]!obMake("","LocalDate",P16),[1]!obMake("","String",Q16),[1]!obMake("","String",R16),$E$8,[1]!obMake("","String",S16),$E$9,[1]!obMake("","int",T16),[1]!obMake("","int",U16)),[1]!obMake("","String",V16),[1]!obMake("","double",W16),[1]!obMake("","boolean",X16),[1]!obMake("","String",Y16),[1]!obMake("","String",Z16))</f>
         <v>cap-16 
-[13135]</v>
+[6234]</v>
       </c>
       <c r="O16" s="31">
         <v>40951</v>
@@ -11405,20 +11438,20 @@
         <v>capletVol</v>
       </c>
       <c r="AB16" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N16,"getValue",$N$10))</f>
-        <v>4.970873666609116E-4</v>
+        <f>[1]!obGet([1]!obCall("",N16,"getValue",$N$10))</f>
+        <v>4.9708608918029552E-4</v>
       </c>
       <c r="AC16" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N16,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
-        <v>0.53195671798775834</v>
+        <f>[1]!obGet([1]!obCall("",N16,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
+        <v>0.5319569649601904</v>
       </c>
     </row>
     <row r="17" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="12"/>
       <c r="N17" s="19" t="str">
-        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!OBCALL("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",O17)),[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",P17)),[1]!obMake("","String",Q17),[1]!obMake("","String",R17),$E$8,[1]!obMake("","String",S17),$E$9,[1]!obMake("","int",T17),[1]!obMake("","int",U17)),[1]!obMake("","String",V17),[1]!obMake("","double",W17),[1]!obMake("","boolean",X17),[1]!obMake("","String",Y17),[1]!obMake("","String",Z17))</f>
+        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!obCall("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("","LocalDate",O17),[1]!obMake("","LocalDate",P17),[1]!obMake("","String",Q17),[1]!obMake("","String",R17),$E$8,[1]!obMake("","String",S17),$E$9,[1]!obMake("","int",T17),[1]!obMake("","int",U17)),[1]!obMake("","String",V17),[1]!obMake("","double",W17),[1]!obMake("","boolean",X17),[1]!obMake("","String",Y17),[1]!obMake("","String",Z17))</f>
         <v>cap-17 
-[13167]</v>
+[6178]</v>
       </c>
       <c r="O17" s="31">
         <v>40920</v>
@@ -11460,12 +11493,12 @@
         <v>capletVol</v>
       </c>
       <c r="AB17" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N17,"getValue",$N$10))</f>
-        <v>1.3317032794445075E-3</v>
+        <f>[1]!obGet([1]!obCall("",N17,"getValue",$N$10))</f>
+        <v>1.3316961482580921E-3</v>
       </c>
       <c r="AC17" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N17,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
-        <v>0.37524423584118222</v>
+        <f>[1]!obGet([1]!obCall("",N17,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
+        <v>0.37524472085035865</v>
       </c>
     </row>
     <row r="18" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -11475,9 +11508,9 @@
       </c>
       <c r="F18" s="14"/>
       <c r="N18" s="19" t="str">
-        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!OBCALL("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",O18)),[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",P18)),[1]!obMake("","String",Q18),[1]!obMake("","String",R18),$E$8,[1]!obMake("","String",S18),$E$9,[1]!obMake("","int",T18),[1]!obMake("","int",U18)),[1]!obMake("","String",V18),[1]!obMake("","double",W18),[1]!obMake("","boolean",X18),[1]!obMake("","String",Y18),[1]!obMake("","String",Z18))</f>
+        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!obCall("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("","LocalDate",O18),[1]!obMake("","LocalDate",P18),[1]!obMake("","String",Q18),[1]!obMake("","String",R18),$E$8,[1]!obMake("","String",S18),$E$9,[1]!obMake("","int",T18),[1]!obMake("","int",U18)),[1]!obMake("","String",V18),[1]!obMake("","double",W18),[1]!obMake("","boolean",X18),[1]!obMake("","String",Y18),[1]!obMake("","String",Z18))</f>
         <v>cap-18 
-[13103]</v>
+[6220]</v>
       </c>
       <c r="O18" s="31">
         <v>40920</v>
@@ -11519,26 +11552,26 @@
         <v>capletVol</v>
       </c>
       <c r="AB18" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N18,"getValue",$N$10))</f>
-        <v>2.6949834741635979E-3</v>
+        <f>[1]!obGet([1]!obCall("",N18,"getValue",$N$10))</f>
+        <v>2.6949663130631141E-3</v>
       </c>
       <c r="AC18" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N18,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
-        <v>0.28357829349289015</v>
+        <f>[1]!obGet([1]!obCall("",N18,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
+        <v>0.28357866512317981</v>
       </c>
     </row>
     <row r="19" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="12"/>
       <c r="E19" s="16" t="str">
-        <f>[1]!OBCALL("schedule",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",F10)),[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",F11)),[1]!obMake("","String",F12),[1]!obMake("","String",F13),$E$8,[1]!obMake("","String",F14),$E$9,[1]!obMake("","int",F15),[1]!obMake("","int",F16))</f>
+        <f>[1]!obCall("schedule",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("","LocalDate",F10),[1]!obMake("","LocalDate",F11),[1]!obMake("","String",F12),[1]!obMake("","String",F13),$E$8,[1]!obMake("","String",F14),$E$9,[1]!obMake("","int",F15),[1]!obMake("","int",F16))</f>
         <v>schedule 
-[13087]</v>
+[6206]</v>
       </c>
       <c r="F19" s="12"/>
       <c r="N19" s="19" t="str">
-        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!OBCALL("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",O19)),[1]!obMake("",obLibs&amp;"org.joda.time.LocalDate",[1]!obMake("","Date",P19)),[1]!obMake("","String",Q19),[1]!obMake("","String",R19),$E$8,[1]!obMake("","String",S19),$E$9,[1]!obMake("","int",T19),[1]!obMake("","int",U19)),[1]!obMake("","String",V19),[1]!obMake("","double",W19),[1]!obMake("","boolean",X19),[1]!obMake("","String",Y19),[1]!obMake("","String",Z19))</f>
+        <f>[1]!obMake("cap-"&amp;ROW(),obLibs&amp;"net.finmath.marketdata.products.Cap",[1]!obCall("",obLibs&amp;"net.finmath.time.ScheduleGenerator","createScheduleFromConventions",$E$7,[1]!obMake("","LocalDate",O19),[1]!obMake("","LocalDate",P19),[1]!obMake("","String",Q19),[1]!obMake("","String",R19),$E$8,[1]!obMake("","String",S19),$E$9,[1]!obMake("","int",T19),[1]!obMake("","int",U19)),[1]!obMake("","String",V19),[1]!obMake("","double",W19),[1]!obMake("","boolean",X19),[1]!obMake("","String",Y19),[1]!obMake("","String",Z19))</f>
         <v>cap-19 
-[13119]</v>
+[6248]</v>
       </c>
       <c r="O19" s="31">
         <v>40920</v>
@@ -11580,12 +11613,12 @@
         <v>capletVol</v>
       </c>
       <c r="AB19" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N19,"getValue",$N$10))</f>
-        <v>5.9127088023978027E-3</v>
+        <f>[1]!obGet([1]!obCall("",N19,"getValue",$N$10))</f>
+        <v>5.9126776161439552E-3</v>
       </c>
       <c r="AC19" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",N19,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
-        <v>0.23546006370551115</v>
+        <f>[1]!obGet([1]!obCall("",N19,"getImpliedVolatility",[1]!obMake("","double",0),$N$10,$AC$12))</f>
+        <v>0.23546027831090943</v>
       </c>
     </row>
     <row r="20" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -11621,14 +11654,14 @@
     </row>
     <row r="30" spans="2:29" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I30" s="16" t="str">
-        <f>[1]!OBCALL("quotingConventionResult "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurfaceInterface$QuotingConvention","valueOf",[1]!obMake("","String",I29))</f>
+        <f>[1]!obCall("quotingConventionResult "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurface$QuotingConvention","valueOf",[1]!obMake("","String",I29))</f>
         <v>quotingConventionResult 9 
-[12984]</v>
+[6129]</v>
       </c>
       <c r="K30" s="16" t="str">
-        <f>[1]!OBCALL("quotingConventionResult "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurfaceInterface$QuotingConvention","valueOf",[1]!obMake("","String",K29))</f>
+        <f>[1]!obCall("quotingConventionResult "&amp;COLUMN(),obLibs&amp;"net.finmath.marketdata.model.volatilities.VolatilitySurface$QuotingConvention","valueOf",[1]!obMake("","String",K29))</f>
         <v>quotingConventionResult 11 
-[13002]</v>
+[6183]</v>
       </c>
       <c r="N30" s="15" t="s">
         <v>90</v>
@@ -11664,7 +11697,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A34)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A34)))</f>
         <v>5.4794520547945206E-3</v>
       </c>
       <c r="C34" s="26">
@@ -11674,12 +11707,12 @@
         <v>0.7</v>
       </c>
       <c r="I34" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B34),[1]!obMake("","double",$C34),I$30))</f>
-        <v>1.6076927960943493E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B34),[1]!obMake("","double",$C34),I$30))</f>
+        <v>1.6076927926980584E-3</v>
       </c>
       <c r="J34" s="27"/>
       <c r="K34" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B34),[1]!obMake("","double",$C34),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B34),[1]!obMake("","double",$C34),K$30))</f>
         <v>1.5503980543576067E-4</v>
       </c>
     </row>
@@ -11688,7 +11721,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A35)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A35)))</f>
         <v>0.25479452054794521</v>
       </c>
       <c r="C35" s="26">
@@ -11698,12 +11731,12 @@
         <v>0.7</v>
       </c>
       <c r="I35" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B35),[1]!obMake("","double",$C35),I$30))</f>
-        <v>1.7137298865663717E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B35),[1]!obMake("","double",$C35),I$30))</f>
+        <v>1.7137298865663713E-3</v>
       </c>
       <c r="J35" s="27"/>
       <c r="K35" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B35),[1]!obMake("","double",$C35),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B35),[1]!obMake("","double",$C35),K$30))</f>
         <v>2.5979208419424555E-4</v>
       </c>
     </row>
@@ -11712,7 +11745,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A36)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A36)))</f>
         <v>0.50410958904109593</v>
       </c>
       <c r="C36" s="26">
@@ -11722,12 +11755,12 @@
         <v>0.7</v>
       </c>
       <c r="I36" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B36),[1]!obMake("","double",$C36),I$30))</f>
-        <v>1.8144388105832553E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B36),[1]!obMake("","double",$C36),I$30))</f>
+        <v>1.8144388105832518E-3</v>
       </c>
       <c r="J36" s="27"/>
       <c r="K36" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B36),[1]!obMake("","double",$C36),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B36),[1]!obMake("","double",$C36),K$30))</f>
         <v>3.6552857307047389E-4</v>
       </c>
     </row>
@@ -11736,7 +11769,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A37)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A37)))</f>
         <v>0.75616438356164384</v>
       </c>
       <c r="C37" s="26">
@@ -11746,12 +11779,12 @@
         <v>0.7</v>
       </c>
       <c r="I37" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B37),[1]!obMake("","double",$C37),I$30))</f>
-        <v>1.9116064479654101E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B37),[1]!obMake("","double",$C37),I$30))</f>
+        <v>1.9116064479654106E-3</v>
       </c>
       <c r="J37" s="27"/>
       <c r="K37" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B37),[1]!obMake("","double",$C37),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B37),[1]!obMake("","double",$C37),K$30))</f>
         <v>4.7673417329034765E-4</v>
       </c>
     </row>
@@ -11760,7 +11793,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A38)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A38)))</f>
         <v>1.0136986301369864</v>
       </c>
       <c r="C38" s="26">
@@ -11770,12 +11803,12 @@
         <v>0.25</v>
       </c>
       <c r="I38" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B38),[1]!obMake("","double",$C38),I$30))</f>
-        <v>7.295502652020973E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B38),[1]!obMake("","double",$C38),I$30))</f>
+        <v>7.2955026520207583E-4</v>
       </c>
       <c r="J38" s="27"/>
       <c r="K38" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B38),[1]!obMake("","double",$C38),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B38),[1]!obMake("","double",$C38),K$30))</f>
         <v>5.2348666547581398E-4</v>
       </c>
     </row>
@@ -11784,7 +11817,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A39)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A39)))</f>
         <v>1.2547945205479452</v>
       </c>
       <c r="C39" s="26">
@@ -11794,13 +11827,13 @@
         <v>0.25</v>
       </c>
       <c r="I39" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B39),[1]!obMake("","double",$C39),I$30))</f>
-        <v>7.63839674514653E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B39),[1]!obMake("","double",$C39),I$30))</f>
+        <v>7.6383967451470027E-4</v>
       </c>
       <c r="J39" s="27"/>
       <c r="K39" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B39),[1]!obMake("","double",$C39),K$30))</f>
-        <v>6.1143652605563214E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B39),[1]!obMake("","double",$C39),K$30))</f>
+        <v>6.1143652605563225E-4</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -11808,7 +11841,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A40)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A40)))</f>
         <v>1.5041095890410958</v>
       </c>
       <c r="C40" s="26">
@@ -11818,12 +11851,12 @@
         <v>0.25</v>
       </c>
       <c r="I40" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B40),[1]!obMake("","double",$C40),I$30))</f>
-        <v>7.9841921622733993E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B40),[1]!obMake("","double",$C40),I$30))</f>
+        <v>7.9841921622732411E-4</v>
       </c>
       <c r="J40" s="27"/>
       <c r="K40" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B40),[1]!obMake("","double",$C40),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B40),[1]!obMake("","double",$C40),K$30))</f>
         <v>7.2540710292093281E-4</v>
       </c>
     </row>
@@ -11832,7 +11865,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A41)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A41)))</f>
         <v>1.7616438356164383</v>
       </c>
       <c r="C41" s="26">
@@ -11842,12 +11875,12 @@
         <v>0.25</v>
       </c>
       <c r="I41" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B41),[1]!obMake("","double",$C41),I$30))</f>
-        <v>8.3384568864824796E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B41),[1]!obMake("","double",$C41),I$30))</f>
+        <v>8.3384568864826444E-4</v>
       </c>
       <c r="J41" s="27"/>
       <c r="K41" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B41),[1]!obMake("","double",$C41),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B41),[1]!obMake("","double",$C41),K$30))</f>
         <v>8.0613654119574094E-4</v>
       </c>
     </row>
@@ -11856,7 +11889,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A42)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A42)))</f>
         <v>2.010958904109589</v>
       </c>
       <c r="C42" s="26">
@@ -11866,12 +11899,12 @@
         <v>0.25</v>
       </c>
       <c r="I42" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B42),[1]!obMake("","double",$C42),I$30))</f>
-        <v>8.8122503606350897E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B42),[1]!obMake("","double",$C42),I$30))</f>
+        <v>8.8122503606352307E-4</v>
       </c>
       <c r="J42" s="27"/>
       <c r="K42" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B42),[1]!obMake("","double",$C42),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B42),[1]!obMake("","double",$C42),K$30))</f>
         <v>9.2720079029476126E-4</v>
       </c>
     </row>
@@ -11880,7 +11913,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A43)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A43)))</f>
         <v>2.2602739726027399</v>
       </c>
       <c r="C43" s="26">
@@ -11890,13 +11923,13 @@
         <v>0.25</v>
       </c>
       <c r="I43" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B43),[1]!obMake("","double",$C43),I$30))</f>
-        <v>9.2785373037971143E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B43),[1]!obMake("","double",$C43),I$30))</f>
+        <v>9.278537303798025E-4</v>
       </c>
       <c r="J43" s="27"/>
       <c r="K43" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B43),[1]!obMake("","double",$C43),K$30))</f>
-        <v>1.058132407053265E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B43),[1]!obMake("","double",$C43),K$30))</f>
+        <v>1.0581324070532653E-3</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -11904,7 +11937,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A44)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A44)))</f>
         <v>2.5095890410958903</v>
       </c>
       <c r="C44" s="26">
@@ -11914,12 +11947,12 @@
         <v>0.2</v>
       </c>
       <c r="I44" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B44),[1]!obMake("","double",$C44),I$30))</f>
-        <v>7.8047390593511149E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B44),[1]!obMake("","double",$C44),I$30))</f>
+        <v>7.8047390593047816E-4</v>
       </c>
       <c r="J44" s="27"/>
       <c r="K44" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B44),[1]!obMake("","double",$C44),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B44),[1]!obMake("","double",$C44),K$30))</f>
         <v>1.2015426467595839E-3</v>
       </c>
     </row>
@@ -11928,7 +11961,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A45)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A45)))</f>
         <v>2.7589041095890412</v>
       </c>
       <c r="C45" s="26">
@@ -11938,12 +11971,12 @@
         <v>0.2</v>
       </c>
       <c r="I45" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B45),[1]!obMake("","double",$C45),I$30))</f>
-        <v>8.1804123514013353E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B45),[1]!obMake("","double",$C45),I$30))</f>
+        <v>8.180412351388533E-4</v>
       </c>
       <c r="J45" s="27"/>
       <c r="K45" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B45),[1]!obMake("","double",$C45),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B45),[1]!obMake("","double",$C45),K$30))</f>
         <v>1.3392638504041608E-3</v>
       </c>
     </row>
@@ -11952,7 +11985,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A46)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A46)))</f>
         <v>3.0082191780821916</v>
       </c>
       <c r="C46" s="26">
@@ -11962,12 +11995,12 @@
         <v>0.2</v>
       </c>
       <c r="I46" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B46),[1]!obMake("","double",$C46),I$30))</f>
-        <v>9.0854143065836261E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B46),[1]!obMake("","double",$C46),I$30))</f>
+        <v>9.0854143065944931E-4</v>
       </c>
       <c r="J46" s="27"/>
       <c r="K46" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B46),[1]!obMake("","double",$C46),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B46),[1]!obMake("","double",$C46),K$30))</f>
         <v>1.6639199205271433E-3</v>
       </c>
     </row>
@@ -11976,7 +12009,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A47)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A47)))</f>
         <v>3.2575342465753425</v>
       </c>
       <c r="C47" s="26">
@@ -11986,12 +12019,12 @@
         <v>0.2</v>
       </c>
       <c r="I47" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B47),[1]!obMake("","double",$C47),I$30))</f>
-        <v>9.9688478673655E-4</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B47),[1]!obMake("","double",$C47),I$30))</f>
+        <v>9.9688478672898639E-4</v>
       </c>
       <c r="J47" s="27"/>
       <c r="K47" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B47),[1]!obMake("","double",$C47),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B47),[1]!obMake("","double",$C47),K$30))</f>
         <v>2.0077943398745949E-3</v>
       </c>
     </row>
@@ -12000,7 +12033,7 @@
         <v>14</v>
       </c>
       <c r="B48" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A48)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A48)))</f>
         <v>3.506849315068493</v>
       </c>
       <c r="C48" s="26">
@@ -12010,12 +12043,12 @@
         <v>0.2</v>
       </c>
       <c r="I48" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B48),[1]!obMake("","double",$C48),I$30))</f>
-        <v>1.0820811467457674E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B48),[1]!obMake("","double",$C48),I$30))</f>
+        <v>1.0820811467120114E-3</v>
       </c>
       <c r="J48" s="27"/>
       <c r="K48" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B48),[1]!obMake("","double",$C48),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B48),[1]!obMake("","double",$C48),K$30))</f>
         <v>2.3754215894831445E-3</v>
       </c>
     </row>
@@ -12024,7 +12057,7 @@
         <v>15</v>
       </c>
       <c r="B49" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A49)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A49)))</f>
         <v>3.7561643835616438</v>
       </c>
       <c r="C49" s="26">
@@ -12034,13 +12067,13 @@
         <v>0.2</v>
       </c>
       <c r="I49" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B49),[1]!obMake("","double",$C49),I$30))</f>
-        <v>1.1638671812229774E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B49),[1]!obMake("","double",$C49),I$30))</f>
+        <v>1.163867181542958E-3</v>
       </c>
       <c r="J49" s="27"/>
       <c r="K49" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B49),[1]!obMake("","double",$C49),K$30))</f>
-        <v>2.7152975712036315E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B49),[1]!obMake("","double",$C49),K$30))</f>
+        <v>2.7152975712036319E-3</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -12048,7 +12081,7 @@
         <v>16</v>
       </c>
       <c r="B50" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A50)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A50)))</f>
         <v>4.0082191780821921</v>
       </c>
       <c r="C50" s="26">
@@ -12058,12 +12091,12 @@
         <v>0.2</v>
       </c>
       <c r="I50" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B50),[1]!obMake("","double",$C50),I$30))</f>
-        <v>1.2098411818486864E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B50),[1]!obMake("","double",$C50),I$30))</f>
+        <v>1.2098411817101432E-3</v>
       </c>
       <c r="J50" s="27"/>
       <c r="K50" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B50),[1]!obMake("","double",$C50),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B50),[1]!obMake("","double",$C50),K$30))</f>
         <v>2.8750848478761781E-3</v>
       </c>
     </row>
@@ -12072,7 +12105,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A51)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A51)))</f>
         <v>4.2575342465753421</v>
       </c>
       <c r="C51" s="26">
@@ -12082,12 +12115,12 @@
         <v>0.2</v>
       </c>
       <c r="I51" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B51),[1]!obMake("","double",$C51),I$30))</f>
-        <v>1.2538825292077373E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B51),[1]!obMake("","double",$C51),I$30))</f>
+        <v>1.2538825290965457E-3</v>
       </c>
       <c r="J51" s="27"/>
       <c r="K51" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B51),[1]!obMake("","double",$C51),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B51),[1]!obMake("","double",$C51),K$30))</f>
         <v>3.0569513813166094E-3</v>
       </c>
     </row>
@@ -12096,7 +12129,7 @@
         <v>18</v>
       </c>
       <c r="B52" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A52)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A52)))</f>
         <v>4.506849315068493</v>
       </c>
       <c r="C52" s="26">
@@ -12106,12 +12139,12 @@
         <v>0.2</v>
       </c>
       <c r="I52" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B52),[1]!obMake("","double",$C52),I$30))</f>
-        <v>1.2973213361832515E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B52),[1]!obMake("","double",$C52),I$30))</f>
+        <v>1.2973213363551795E-3</v>
       </c>
       <c r="J52" s="27"/>
       <c r="K52" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B52),[1]!obMake("","double",$C52),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B52),[1]!obMake("","double",$C52),K$30))</f>
         <v>3.2721491262059877E-3</v>
       </c>
     </row>
@@ -12120,7 +12153,7 @@
         <v>19</v>
       </c>
       <c r="B53" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A53)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A53)))</f>
         <v>4.7589041095890412</v>
       </c>
       <c r="C53" s="26">
@@ -12130,12 +12163,12 @@
         <v>0.2</v>
       </c>
       <c r="I53" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B53),[1]!obMake("","double",$C53),I$30))</f>
-        <v>1.3414220796630076E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B53),[1]!obMake("","double",$C53),I$30))</f>
+        <v>1.3414220796158787E-3</v>
       </c>
       <c r="J53" s="27"/>
       <c r="K53" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B53),[1]!obMake("","double",$C53),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B53),[1]!obMake("","double",$C53),K$30))</f>
         <v>3.4569510225920014E-3</v>
       </c>
     </row>
@@ -12144,7 +12177,7 @@
         <v>20</v>
       </c>
       <c r="B54" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A54)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A54)))</f>
         <v>5.0109589041095894</v>
       </c>
       <c r="C54" s="26">
@@ -12154,12 +12187,12 @@
         <v>0.2</v>
       </c>
       <c r="I54" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B54),[1]!obMake("","double",$C54),I$30))</f>
-        <v>1.4091037024615352E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B54),[1]!obMake("","double",$C54),I$30))</f>
+        <v>1.4091037027605126E-3</v>
       </c>
       <c r="J54" s="27"/>
       <c r="K54" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B54),[1]!obMake("","double",$C54),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B54),[1]!obMake("","double",$C54),K$30))</f>
         <v>3.6665856059975663E-3</v>
       </c>
     </row>
@@ -12168,7 +12201,7 @@
         <v>21</v>
       </c>
       <c r="B55" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A55)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A55)))</f>
         <v>5.2575342465753421</v>
       </c>
       <c r="C55" s="26">
@@ -12178,13 +12211,13 @@
         <v>0.2</v>
       </c>
       <c r="I55" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B55),[1]!obMake("","double",$C55),I$30))</f>
-        <v>1.4748846880929312E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B55),[1]!obMake("","double",$C55),I$30))</f>
+        <v>1.4748846874264936E-3</v>
       </c>
       <c r="J55" s="27"/>
       <c r="K55" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B55),[1]!obMake("","double",$C55),K$30))</f>
-        <v>3.9885953080421952E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B55),[1]!obMake("","double",$C55),K$30))</f>
+        <v>3.9885953080421943E-3</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -12192,7 +12225,7 @@
         <v>22</v>
       </c>
       <c r="B56" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A56)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A56)))</f>
         <v>5.506849315068493</v>
       </c>
       <c r="C56" s="26">
@@ -12202,12 +12235,12 @@
         <v>0.2</v>
       </c>
       <c r="I56" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B56),[1]!obMake("","double",$C56),I$30))</f>
-        <v>1.5403274995156248E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B56),[1]!obMake("","double",$C56),I$30))</f>
+        <v>1.540327499877656E-3</v>
       </c>
       <c r="J56" s="27"/>
       <c r="K56" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B56),[1]!obMake("","double",$C56),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B56),[1]!obMake("","double",$C56),K$30))</f>
         <v>4.3166083757098716E-3</v>
       </c>
     </row>
@@ -12216,7 +12249,7 @@
         <v>23</v>
       </c>
       <c r="B57" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A57)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A57)))</f>
         <v>5.7589041095890412</v>
       </c>
       <c r="C57" s="26">
@@ -12226,12 +12259,12 @@
         <v>0.2</v>
       </c>
       <c r="I57" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B57),[1]!obMake("","double",$C57),I$30))</f>
-        <v>2.0344989698222395E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B57),[1]!obMake("","double",$C57),I$30))</f>
+        <v>2.0344989698218574E-3</v>
       </c>
       <c r="J57" s="27"/>
       <c r="K57" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B57),[1]!obMake("","double",$C57),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B57),[1]!obMake("","double",$C57),K$30))</f>
         <v>4.1119009869960647E-3</v>
       </c>
     </row>
@@ -12240,7 +12273,7 @@
         <v>24</v>
       </c>
       <c r="B58" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A58)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A58)))</f>
         <v>6.0109589041095894</v>
       </c>
       <c r="C58" s="26">
@@ -12250,12 +12283,12 @@
         <v>0.2</v>
       </c>
       <c r="I58" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B58),[1]!obMake("","double",$C58),I$30))</f>
-        <v>2.0543687111110377E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B58),[1]!obMake("","double",$C58),I$30))</f>
+        <v>2.054368711108714E-3</v>
       </c>
       <c r="J58" s="27"/>
       <c r="K58" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B58),[1]!obMake("","double",$C58),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B58),[1]!obMake("","double",$C58),K$30))</f>
         <v>4.0836058695249838E-3</v>
       </c>
     </row>
@@ -12264,7 +12297,7 @@
         <v>25</v>
       </c>
       <c r="B59" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A59)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A59)))</f>
         <v>6.2575342465753421</v>
       </c>
       <c r="C59" s="26">
@@ -12274,12 +12307,12 @@
         <v>0.2</v>
       </c>
       <c r="I59" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B59),[1]!obMake("","double",$C59),I$30))</f>
-        <v>2.072078526859901E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B59),[1]!obMake("","double",$C59),I$30))</f>
+        <v>2.0720785268603841E-3</v>
       </c>
       <c r="J59" s="27"/>
       <c r="K59" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B59),[1]!obMake("","double",$C59),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B59),[1]!obMake("","double",$C59),K$30))</f>
         <v>4.1811352651209052E-3</v>
       </c>
     </row>
@@ -12288,7 +12321,7 @@
         <v>26</v>
       </c>
       <c r="B60" s="16">
-        <f>[1]!OBGET([1]!OBCALL("",$E$19,"getFixing",[1]!obMake("","int",A60)))</f>
+        <f>[1]!obGet([1]!obCall("",$E$19,"getFixing",[1]!obMake("","int",A60)))</f>
         <v>6.506849315068493</v>
       </c>
       <c r="C60" s="26">
@@ -12298,18 +12331,143 @@
         <v>0.2</v>
       </c>
       <c r="I60" s="26">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B60),[1]!obMake("","double",$C60),I$30))</f>
-        <v>2.0899051353278058E-3</v>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B60),[1]!obMake("","double",$C60),I$30))</f>
+        <v>2.0899051353282989E-3</v>
       </c>
       <c r="J60" s="27"/>
       <c r="K60" s="36">
-        <f>[1]!OBGET([1]!OBCALL("",$B$14,"getValue",[1]!obMake("","double",$B60),[1]!obMake("","double",$C60),K$30))</f>
+        <f>[1]!obGet([1]!obCall("",$B$14,"getValue",[1]!obMake("","double",$B60),[1]!obMake("","double",$C60),K$30))</f>
         <v>4.2790364797850944E-3</v>
       </c>
+    </row>
+    <row r="61" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+    </row>
+    <row r="62" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="27"/>
+      <c r="J62" s="27"/>
+      <c r="K62" s="27"/>
+    </row>
+    <row r="63" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="27"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="27"/>
+    </row>
+    <row r="64" spans="1:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+    </row>
+    <row r="65" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" s="27"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+    </row>
+    <row r="66" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I66" s="27"/>
+      <c r="J66" s="27"/>
+      <c r="K66" s="27"/>
+    </row>
+    <row r="67" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" s="27"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+    </row>
+    <row r="68" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I68" s="27"/>
+      <c r="J68" s="27"/>
+      <c r="K68" s="27"/>
+    </row>
+    <row r="69" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+    </row>
+    <row r="70" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="27"/>
+      <c r="J70" s="27"/>
+      <c r="K70" s="27"/>
+    </row>
+    <row r="71" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I71" s="27"/>
+      <c r="J71" s="27"/>
+      <c r="K71" s="27"/>
+    </row>
+    <row r="72" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="27"/>
+      <c r="J72" s="27"/>
+      <c r="K72" s="27"/>
+    </row>
+    <row r="73" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="27"/>
+      <c r="J73" s="27"/>
+      <c r="K73" s="27"/>
+    </row>
+    <row r="74" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I74" s="27"/>
+      <c r="J74" s="27"/>
+      <c r="K74" s="27"/>
+    </row>
+    <row r="75" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I75" s="27"/>
+      <c r="J75" s="27"/>
+      <c r="K75" s="27"/>
+    </row>
+    <row r="76" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="27"/>
+      <c r="J76" s="27"/>
+      <c r="K76" s="27"/>
+    </row>
+    <row r="77" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I77" s="27"/>
+      <c r="J77" s="27"/>
+      <c r="K77" s="27"/>
+    </row>
+    <row r="78" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I78" s="27"/>
+      <c r="J78" s="27"/>
+      <c r="K78" s="27"/>
+    </row>
+    <row r="79" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I79" s="27"/>
+      <c r="J79" s="27"/>
+      <c r="K79" s="27"/>
+    </row>
+    <row r="80" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I80" s="27"/>
+      <c r="J80" s="27"/>
+      <c r="K80" s="27"/>
+    </row>
+    <row r="81" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I81" s="27"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="27"/>
+    </row>
+    <row r="82" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I82" s="27"/>
+      <c r="J82" s="27"/>
+      <c r="K82" s="27"/>
+    </row>
+    <row r="83" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I83" s="27"/>
+      <c r="J83" s="27"/>
+      <c r="K83" s="27"/>
+    </row>
+    <row r="84" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I84" s="27"/>
+      <c r="J84" s="27"/>
+      <c r="K84" s="27"/>
+    </row>
+    <row r="85" spans="9:11" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="27"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>

</xml_diff>